<commit_message>
Create an updated menu file with all available categories
Generate a new Excel file containing 91 menu items across 38 database categories, following the specified template format with columns for Name, Description, Price, Category, IsVeg, Image, and IsAvailable.

Replit-Commit-Author: Agent
Replit-Commit-Session-Id: d5825b2d-5a70-4950-bc3e-e69072dc9210
Replit-Commit-Checkpoint-Type: full_checkpoint
Replit-Commit-Event-Id: f4525183-ca28-415e-9436-de6521f1a106
Replit-Commit-Screenshot-Url: https://storage.googleapis.com/screenshot-production-us-central1/a0e76cf1-50a4-4033-88e9-413827fbeca2/d5825b2d-5a70-4950-bc3e-e69072dc9210/hllg6Je
Replit-Helium-Checkpoint-Created: true
</commit_message>
<xml_diff>
--- a/BarrelBorn_Menu_Template.xlsx
+++ b/BarrelBorn_Menu_Template.xlsx
@@ -397,15 +397,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G72"/>
+  <dimension ref="A1:G92"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <cols>
-    <col min="1" max="1" width="25.83203125" customWidth="1"/>
-    <col min="2" max="2" width="45.83203125" customWidth="1"/>
+    <col min="1" max="1" width="28.83203125" customWidth="1"/>
+    <col min="2" max="2" width="50.83203125" customWidth="1"/>
     <col min="3" max="3" width="20.83203125" customWidth="1"/>
-    <col min="4" max="4" width="25.83203125" customWidth="1"/>
+    <col min="4" max="4" width="28.83203125" customWidth="1"/>
     <col min="5" max="5" width="10.83203125" customWidth="1"/>
     <col min="6" max="6" width="30.83203125" customWidth="1"/>
     <col min="7" max="7" width="12.83203125" customWidth="1"/>
@@ -436,16 +436,16 @@
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>Gateway White Zen</v>
+        <v>Samosa (2 pcs)</v>
       </c>
       <c r="B2" t="str">
-        <v>Light German Style Wheat Beer</v>
+        <v>Crispy potato &amp; pea pastry</v>
       </c>
       <c r="C2" t="str">
-        <v>265 / 485 / 1350</v>
+        <v>120</v>
       </c>
       <c r="D2" t="str">
-        <v>craft-beers-on-tap</v>
+        <v>nibbles</v>
       </c>
       <c r="E2" t="b">
         <v>1</v>
@@ -459,16 +459,16 @@
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v>Gateway Doppelganger</v>
+        <v>Paneer Tikka Masala</v>
       </c>
       <c r="B3" t="str">
-        <v>Smooth German-style Coffee Stout</v>
+        <v>Cottage cheese cubes in creamy tomato gravy</v>
       </c>
       <c r="C3" t="str">
-        <v>265 / 485 / 1350</v>
+        <v>249</v>
       </c>
       <c r="D3" t="str">
-        <v>craft-beers-on-tap</v>
+        <v>starters</v>
       </c>
       <c r="E3" t="b">
         <v>1</v>
@@ -482,19 +482,19 @@
     </row>
     <row r="4">
       <c r="A4" t="str">
-        <v>Bira 91 Pilsner</v>
+        <v>Chicken Biryani</v>
       </c>
       <c r="B4" t="str">
-        <v>Crisp, refreshing, easy-drinking</v>
+        <v>Aromatic basmati rice cooked with tender chicken</v>
       </c>
       <c r="C4" t="str">
-        <v>235 / 410 / 1195</v>
+        <v>299</v>
       </c>
       <c r="D4" t="str">
-        <v>craft-beers-on-tap</v>
+        <v>biryani</v>
       </c>
       <c r="E4" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F4" t="str">
         <v/>
@@ -505,16 +505,16 @@
     </row>
     <row r="5">
       <c r="A5" t="str">
-        <v>Bira 91 Belgian Golden Strong Ale</v>
+        <v>Paneer Butter Masala</v>
       </c>
       <c r="B5" t="str">
-        <v>Fruity, Belgian-style</v>
+        <v>Soft paneer cubes in rich butter sauce</v>
       </c>
       <c r="C5" t="str">
-        <v>235 / 410 / 1195</v>
+        <v>249</v>
       </c>
       <c r="D5" t="str">
-        <v>craft-beers-on-tap</v>
+        <v>entree</v>
       </c>
       <c r="E5" t="b">
         <v>1</v>
@@ -528,19 +528,19 @@
     </row>
     <row r="6">
       <c r="A6" t="str">
-        <v>Bira 91 WC IPA</v>
+        <v>Butter Chicken</v>
       </c>
       <c r="B6" t="str">
-        <v>Hoppy, bold &amp; aromatic</v>
+        <v>Tender chicken in creamy tomato sauce</v>
       </c>
       <c r="C6" t="str">
-        <v>235 / 410 / 1195</v>
+        <v>279</v>
       </c>
       <c r="D6" t="str">
-        <v>craft-beers-on-tap</v>
+        <v>entree</v>
       </c>
       <c r="E6" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F6" t="str">
         <v/>
@@ -551,16 +551,16 @@
     </row>
     <row r="7">
       <c r="A7" t="str">
-        <v>Bira 91 Hefeweizen</v>
+        <v>Butter Naan</v>
       </c>
       <c r="B7" t="str">
-        <v>Smooth wheat beer with banana &amp; clove notes</v>
+        <v>Soft Indian bread brushed with butter</v>
       </c>
       <c r="C7" t="str">
-        <v>235 / 410 / 1195</v>
+        <v>80</v>
       </c>
       <c r="D7" t="str">
-        <v>craft-beers-on-tap</v>
+        <v>breads</v>
       </c>
       <c r="E7" t="b">
         <v>1</v>
@@ -574,16 +574,16 @@
     </row>
     <row r="8">
       <c r="A8" t="str">
-        <v>Drifter Basmati</v>
+        <v>Garlic Naan</v>
       </c>
       <c r="B8" t="str">
-        <v>Unique basmati aroma, super smooth</v>
+        <v>Naan topped with garlic &amp; herbs</v>
       </c>
       <c r="C8" t="str">
-        <v>245 / 460 / 1330</v>
+        <v>90</v>
       </c>
       <c r="D8" t="str">
-        <v>craft-beers-on-tap</v>
+        <v>breads</v>
       </c>
       <c r="E8" t="b">
         <v>1</v>
@@ -597,16 +597,16 @@
     </row>
     <row r="9">
       <c r="A9" t="str">
-        <v>Drifter Cream Stout</v>
+        <v>Dal Makhani</v>
       </c>
       <c r="B9" t="str">
-        <v>Dark, creamy, chocolate &amp; coffee notes</v>
+        <v>Creamy black lentil preparation</v>
       </c>
       <c r="C9" t="str">
-        <v>245 / 460 / 1330</v>
+        <v>199</v>
       </c>
       <c r="D9" t="str">
-        <v>craft-beers-on-tap</v>
+        <v>dals</v>
       </c>
       <c r="E9" t="b">
         <v>1</v>
@@ -620,19 +620,19 @@
     </row>
     <row r="10">
       <c r="A10" t="str">
-        <v>Drifter Kokam Cider</v>
+        <v>Tandoori Chicken</v>
       </c>
       <c r="B10" t="str">
-        <v>Tart, fruity cider with coastal kokam</v>
+        <v>Grilled chicken marinated in yogurt &amp; spices</v>
       </c>
       <c r="C10" t="str">
-        <v>245 / 460 / 1330</v>
+        <v>249</v>
       </c>
       <c r="D10" t="str">
-        <v>craft-beers-on-tap</v>
+        <v>charcoal</v>
       </c>
       <c r="E10" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F10" t="str">
         <v/>
@@ -643,16 +643,16 @@
     </row>
     <row r="11">
       <c r="A11" t="str">
-        <v>Kingfisher Draught</v>
+        <v>Paneer Tikka</v>
       </c>
       <c r="B11" t="str">
-        <v>Classic, smooth, perfect for sessions</v>
+        <v>Marinated paneer grilled in tandoor</v>
       </c>
       <c r="C11" t="str">
-        <v>255 / 375 / 995</v>
+        <v>219</v>
       </c>
       <c r="D11" t="str">
-        <v>draught-beer</v>
+        <v>charcoal</v>
       </c>
       <c r="E11" t="b">
         <v>1</v>
@@ -666,19 +666,19 @@
     </row>
     <row r="12">
       <c r="A12" t="str">
-        <v>Hoegaarden</v>
+        <v>Pasta Carbonara</v>
       </c>
       <c r="B12" t="str">
-        <v>Belgian wheat beer – smooth &amp; citrusy</v>
+        <v>Creamy pasta with bacon &amp; parmesan</v>
       </c>
       <c r="C12" t="str">
-        <v>495</v>
+        <v>249</v>
       </c>
       <c r="D12" t="str">
-        <v>pint-beers</v>
+        <v>pasta</v>
       </c>
       <c r="E12" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F12" t="str">
         <v/>
@@ -689,16 +689,16 @@
     </row>
     <row r="13">
       <c r="A13" t="str">
-        <v>Corona</v>
+        <v>Margherita Pizza</v>
       </c>
       <c r="B13" t="str">
-        <v>Light &amp; crisp — best with lime</v>
+        <v>Fresh mozzarella, tomato &amp; basil on thin crust</v>
       </c>
       <c r="C13" t="str">
-        <v>495</v>
+        <v>249</v>
       </c>
       <c r="D13" t="str">
-        <v>pint-beers</v>
+        <v>pizza</v>
       </c>
       <c r="E13" t="b">
         <v>1</v>
@@ -712,19 +712,19 @@
     </row>
     <row r="14">
       <c r="A14" t="str">
-        <v>Kingfisher Strong</v>
+        <v>Chicken Slider</v>
       </c>
       <c r="B14" t="str">
-        <v>Strong &amp; popular lager</v>
+        <v>Grilled chicken burger on soft roll</v>
       </c>
       <c r="C14" t="str">
-        <v>375</v>
+        <v>149</v>
       </c>
       <c r="D14" t="str">
-        <v>pint-beers</v>
+        <v>sliders</v>
       </c>
       <c r="E14" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F14" t="str">
         <v/>
@@ -735,19 +735,19 @@
     </row>
     <row r="15">
       <c r="A15" t="str">
-        <v>Budweiser Magnum</v>
+        <v>Thai Green Curry</v>
       </c>
       <c r="B15" t="str">
-        <v>Strong &amp; popular lager</v>
+        <v>Aromatic green curry with chicken &amp; vegetables</v>
       </c>
       <c r="C15" t="str">
-        <v>435</v>
+        <v>279</v>
       </c>
       <c r="D15" t="str">
-        <v>pint-beers</v>
+        <v>thai-bowls</v>
       </c>
       <c r="E15" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F15" t="str">
         <v/>
@@ -758,19 +758,19 @@
     </row>
     <row r="16">
       <c r="A16" t="str">
-        <v>Carlsberg Elephant</v>
+        <v>Rice Noodles with Shrimp</v>
       </c>
       <c r="B16" t="str">
-        <v>Strong &amp; popular lager</v>
+        <v>Stir-fried rice noodles with fresh shrimp</v>
       </c>
       <c r="C16" t="str">
-        <v>375</v>
+        <v>299</v>
       </c>
       <c r="D16" t="str">
-        <v>pint-beers</v>
+        <v>rice-noodles</v>
       </c>
       <c r="E16" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F16" t="str">
         <v/>
@@ -781,16 +781,16 @@
     </row>
     <row r="17">
       <c r="A17" t="str">
-        <v>Budweiser</v>
+        <v>Vegetable Sizzler</v>
       </c>
       <c r="B17" t="str">
-        <v>Easy drinking lager</v>
+        <v>Grilled seasonal vegetables on hot plate</v>
       </c>
       <c r="C17" t="str">
-        <v>345</v>
+        <v>249</v>
       </c>
       <c r="D17" t="str">
-        <v>pint-beers</v>
+        <v>sizzlers</v>
       </c>
       <c r="E17" t="b">
         <v>1</v>
@@ -804,19 +804,19 @@
     </row>
     <row r="18">
       <c r="A18" t="str">
-        <v>Amstel Light</v>
+        <v>Chicken Sizzler</v>
       </c>
       <c r="B18" t="str">
-        <v>Easy drinking lager</v>
+        <v>Grilled chicken strips on hot plate</v>
       </c>
       <c r="C18" t="str">
-        <v>375</v>
+        <v>349</v>
       </c>
       <c r="D18" t="str">
-        <v>pint-beers</v>
+        <v>sizzlers</v>
       </c>
       <c r="E18" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F18" t="str">
         <v/>
@@ -827,19 +827,19 @@
     </row>
     <row r="19">
       <c r="A19" t="str">
-        <v>Carlsberg Smooth</v>
+        <v>Dim Sum Platter</v>
       </c>
       <c r="B19" t="str">
-        <v>Easy drinking lager</v>
+        <v>Assorted steamed dumplings with dipping sauces</v>
       </c>
       <c r="C19" t="str">
-        <v>345</v>
+        <v>299</v>
       </c>
       <c r="D19" t="str">
-        <v>pint-beers</v>
+        <v>bao-dimsum</v>
       </c>
       <c r="E19" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F19" t="str">
         <v/>
@@ -850,16 +850,16 @@
     </row>
     <row r="20">
       <c r="A20" t="str">
-        <v>Heineken</v>
+        <v>Paneer Curry</v>
       </c>
       <c r="B20" t="str">
-        <v>Easy drinking lager</v>
+        <v>Paneer in aromatic curry sauce</v>
       </c>
       <c r="C20" t="str">
-        <v>345</v>
+        <v>229</v>
       </c>
       <c r="D20" t="str">
-        <v>pint-beers</v>
+        <v>curries</v>
       </c>
       <c r="E20" t="b">
         <v>1</v>
@@ -873,19 +873,19 @@
     </row>
     <row r="21">
       <c r="A21" t="str">
-        <v>KF Mild</v>
+        <v>Chicken Curry</v>
       </c>
       <c r="B21" t="str">
-        <v>Value friendly pick</v>
+        <v>Tender chicken in rich gravy</v>
       </c>
       <c r="C21" t="str">
-        <v>275</v>
+        <v>249</v>
       </c>
       <c r="D21" t="str">
-        <v>pint-beers</v>
+        <v>curries</v>
       </c>
       <c r="E21" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F21" t="str">
         <v/>
@@ -896,16 +896,16 @@
     </row>
     <row r="22">
       <c r="A22" t="str">
-        <v>KF Ultra</v>
+        <v>Vegetable Biryani</v>
       </c>
       <c r="B22" t="str">
-        <v>Value friendly pick</v>
+        <v>Aromatic rice with mixed vegetables</v>
       </c>
       <c r="C22" t="str">
-        <v>325</v>
+        <v>229</v>
       </c>
       <c r="D22" t="str">
-        <v>pint-beers</v>
+        <v>biryani</v>
       </c>
       <c r="E22" t="b">
         <v>1</v>
@@ -919,16 +919,16 @@
     </row>
     <row r="23">
       <c r="A23" t="str">
-        <v>Tuborg Green</v>
+        <v>Lentil Soup</v>
       </c>
       <c r="B23" t="str">
-        <v>Value friendly pick</v>
+        <v>Creamy lentil &amp; vegetable soup</v>
       </c>
       <c r="C23" t="str">
-        <v>325</v>
+        <v>149</v>
       </c>
       <c r="D23" t="str">
-        <v>pint-beers</v>
+        <v>soups</v>
       </c>
       <c r="E23" t="b">
         <v>1</v>
@@ -942,19 +942,19 @@
     </row>
     <row r="24">
       <c r="A24" t="str">
-        <v>Tuborg</v>
+        <v>Chicken Soup</v>
       </c>
       <c r="B24" t="str">
-        <v>Value friendly pick</v>
+        <v>Light broth with chicken &amp; vegetables</v>
       </c>
       <c r="C24" t="str">
-        <v>325</v>
+        <v>169</v>
       </c>
       <c r="D24" t="str">
-        <v>pint-beers</v>
+        <v>soups</v>
       </c>
       <c r="E24" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F24" t="str">
         <v/>
@@ -965,16 +965,16 @@
     </row>
     <row r="25">
       <c r="A25" t="str">
-        <v>Peoples Lager</v>
+        <v>Rocket &amp; Parmesan Salad</v>
       </c>
       <c r="B25" t="str">
-        <v>Local craft-style lager</v>
+        <v>Fresh arugula with shaved parmesan &amp; balsamic</v>
       </c>
       <c r="C25" t="str">
-        <v>405</v>
+        <v>199</v>
       </c>
       <c r="D25" t="str">
-        <v>pint-beers</v>
+        <v>salads</v>
       </c>
       <c r="E25" t="b">
         <v>1</v>
@@ -988,19 +988,19 @@
     </row>
     <row r="26">
       <c r="A26" t="str">
-        <v>Breezer</v>
+        <v>Grilled Chicken Salad</v>
       </c>
       <c r="B26" t="str">
-        <v>Fruity, refreshing, low-alcohol</v>
+        <v>Mixed greens with grilled chicken strips</v>
       </c>
       <c r="C26" t="str">
-        <v>350</v>
+        <v>249</v>
       </c>
       <c r="D26" t="str">
-        <v>pint-beers</v>
+        <v>salads</v>
       </c>
       <c r="E26" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F26" t="str">
         <v/>
@@ -1011,19 +1011,19 @@
     </row>
     <row r="27">
       <c r="A27" t="str">
-        <v>LIIT</v>
+        <v>Asian Noodles</v>
       </c>
       <c r="B27" t="str">
-        <v>Powerful blend of five white spirits, citrus, and cola</v>
+        <v>Stir-fried noodles with Asian flavors</v>
       </c>
       <c r="C27" t="str">
-        <v>800</v>
+        <v>229</v>
       </c>
       <c r="D27" t="str">
-        <v>classic-cocktails</v>
+        <v>asian-mains</v>
       </c>
       <c r="E27" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F27" t="str">
         <v/>
@@ -1034,16 +1034,16 @@
     </row>
     <row r="28">
       <c r="A28" t="str">
-        <v>Mojito</v>
+        <v>Gateway White Zen</v>
       </c>
       <c r="B28" t="str">
-        <v>Fresh mint, lime, sugar, and white rum topped with soda</v>
+        <v>Light German Style Wheat Beer</v>
       </c>
       <c r="C28" t="str">
-        <v>450</v>
+        <v>265 / 485 / 1350</v>
       </c>
       <c r="D28" t="str">
-        <v>classic-cocktails</v>
+        <v>craft-beers-on-tap</v>
       </c>
       <c r="E28" t="b">
         <v>1</v>
@@ -1057,16 +1057,16 @@
     </row>
     <row r="29">
       <c r="A29" t="str">
-        <v>Martini</v>
+        <v>Gateway Doppelganger</v>
       </c>
       <c r="B29" t="str">
-        <v>Gin or vodka with dry vermouth</v>
+        <v>Smooth German-style Coffee Stout</v>
       </c>
       <c r="C29" t="str">
-        <v>450</v>
+        <v>265 / 485 / 1350</v>
       </c>
       <c r="D29" t="str">
-        <v>classic-cocktails</v>
+        <v>craft-beers-on-tap</v>
       </c>
       <c r="E29" t="b">
         <v>1</v>
@@ -1080,16 +1080,16 @@
     </row>
     <row r="30">
       <c r="A30" t="str">
-        <v>Manhattan</v>
+        <v>Bira 91 Pilsner</v>
       </c>
       <c r="B30" t="str">
-        <v>Whisky stirred with sweet vermouth &amp; bitters</v>
+        <v>Crisp, refreshing, easy-drinking</v>
       </c>
       <c r="C30" t="str">
-        <v>450</v>
+        <v>235 / 410 / 1195</v>
       </c>
       <c r="D30" t="str">
-        <v>classic-cocktails</v>
+        <v>craft-beers-on-tap</v>
       </c>
       <c r="E30" t="b">
         <v>1</v>
@@ -1103,16 +1103,16 @@
     </row>
     <row r="31">
       <c r="A31" t="str">
-        <v>Cosmopolitan</v>
+        <v>Bira 91 Belgian Golden Strong Ale</v>
       </c>
       <c r="B31" t="str">
-        <v>Vodka, cranberry, lime &amp; triple sec</v>
+        <v>Fruity, Belgian-style</v>
       </c>
       <c r="C31" t="str">
-        <v>450</v>
+        <v>235 / 410 / 1195</v>
       </c>
       <c r="D31" t="str">
-        <v>classic-cocktails</v>
+        <v>craft-beers-on-tap</v>
       </c>
       <c r="E31" t="b">
         <v>1</v>
@@ -1126,16 +1126,16 @@
     </row>
     <row r="32">
       <c r="A32" t="str">
-        <v>Pina Colada</v>
+        <v>Bira 91 WC IPA</v>
       </c>
       <c r="B32" t="str">
-        <v>Pineapple, coconut cream &amp; rum</v>
+        <v>Hoppy, bold &amp; aromatic</v>
       </c>
       <c r="C32" t="str">
-        <v>450</v>
+        <v>235 / 410 / 1195</v>
       </c>
       <c r="D32" t="str">
-        <v>classic-cocktails</v>
+        <v>craft-beers-on-tap</v>
       </c>
       <c r="E32" t="b">
         <v>1</v>
@@ -1149,16 +1149,16 @@
     </row>
     <row r="33">
       <c r="A33" t="str">
-        <v>Margarita</v>
+        <v>Drifter Basmati</v>
       </c>
       <c r="B33" t="str">
-        <v>Tequila, lime &amp; triple sec with a salted rim</v>
+        <v>Unique basmati aroma, super smooth</v>
       </c>
       <c r="C33" t="str">
-        <v>450</v>
+        <v>245 / 460 / 1330</v>
       </c>
       <c r="D33" t="str">
-        <v>classic-cocktails</v>
+        <v>craft-beers-on-tap</v>
       </c>
       <c r="E33" t="b">
         <v>1</v>
@@ -1172,16 +1172,16 @@
     </row>
     <row r="34">
       <c r="A34" t="str">
-        <v>Moscow Mule</v>
+        <v>Drifter Cream Stout</v>
       </c>
       <c r="B34" t="str">
-        <v>Vodka, ginger beer &amp; lime served cold</v>
+        <v>Dark, creamy, chocolate &amp; coffee notes</v>
       </c>
       <c r="C34" t="str">
-        <v>450</v>
+        <v>245 / 460 / 1330</v>
       </c>
       <c r="D34" t="str">
-        <v>classic-cocktails</v>
+        <v>craft-beers-on-tap</v>
       </c>
       <c r="E34" t="b">
         <v>1</v>
@@ -1195,16 +1195,16 @@
     </row>
     <row r="35">
       <c r="A35" t="str">
-        <v>Old Fashioned</v>
+        <v>Kingfisher Draught</v>
       </c>
       <c r="B35" t="str">
-        <v>Whisky, bitter &amp; sugar, stirred on ice</v>
+        <v>Classic, smooth, perfect for sessions</v>
       </c>
       <c r="C35" t="str">
-        <v>450</v>
+        <v>255 / 375 / 995</v>
       </c>
       <c r="D35" t="str">
-        <v>classic-cocktails</v>
+        <v>draught-beer</v>
       </c>
       <c r="E35" t="b">
         <v>1</v>
@@ -1218,16 +1218,16 @@
     </row>
     <row r="36">
       <c r="A36" t="str">
-        <v>Bloody Mary</v>
+        <v>Hoegaarden</v>
       </c>
       <c r="B36" t="str">
-        <v>Vodka, tomato juice, spice blend &amp; lemon</v>
+        <v>Belgian wheat beer – smooth &amp; citrusy</v>
       </c>
       <c r="C36" t="str">
-        <v>450</v>
+        <v>495</v>
       </c>
       <c r="D36" t="str">
-        <v>classic-cocktails</v>
+        <v>pint-beers</v>
       </c>
       <c r="E36" t="b">
         <v>1</v>
@@ -1241,16 +1241,16 @@
     </row>
     <row r="37">
       <c r="A37" t="str">
-        <v>Picante</v>
+        <v>Corona</v>
       </c>
       <c r="B37" t="str">
-        <v>Tequila, lime &amp; chilli with a herbal twist</v>
+        <v>Light &amp; crisp — best with lime</v>
       </c>
       <c r="C37" t="str">
-        <v>650</v>
+        <v>495</v>
       </c>
       <c r="D37" t="str">
-        <v>classic-cocktails</v>
+        <v>pint-beers</v>
       </c>
       <c r="E37" t="b">
         <v>1</v>
@@ -1264,16 +1264,16 @@
     </row>
     <row r="38">
       <c r="A38" t="str">
-        <v>Espresso Martini</v>
+        <v>Budweiser</v>
       </c>
       <c r="B38" t="str">
-        <v>Vodka, coffee &amp; coffee liqueur</v>
+        <v>Easy drinking lager</v>
       </c>
       <c r="C38" t="str">
-        <v>450</v>
+        <v>345</v>
       </c>
       <c r="D38" t="str">
-        <v>classic-cocktails</v>
+        <v>pint-beers</v>
       </c>
       <c r="E38" t="b">
         <v>1</v>
@@ -1287,16 +1287,16 @@
     </row>
     <row r="39">
       <c r="A39" t="str">
-        <v>Daiquiri</v>
+        <v>Heineken</v>
       </c>
       <c r="B39" t="str">
-        <v>Rum, lime &amp; sugar shaken crisp</v>
+        <v>Premium pilsner lager</v>
       </c>
       <c r="C39" t="str">
-        <v>450</v>
+        <v>345</v>
       </c>
       <c r="D39" t="str">
-        <v>classic-cocktails</v>
+        <v>pint-beers</v>
       </c>
       <c r="E39" t="b">
         <v>1</v>
@@ -1310,10 +1310,10 @@
     </row>
     <row r="40">
       <c r="A40" t="str">
-        <v>Negroni</v>
+        <v>Mojito</v>
       </c>
       <c r="B40" t="str">
-        <v>Gin, sweet vermouth &amp; bitters</v>
+        <v>Fresh mint, lime, sugar, and white rum topped with soda</v>
       </c>
       <c r="C40" t="str">
         <v>450</v>
@@ -1333,10 +1333,10 @@
     </row>
     <row r="41">
       <c r="A41" t="str">
-        <v>Sidecar</v>
+        <v>Martini</v>
       </c>
       <c r="B41" t="str">
-        <v>Brandy, triple sec &amp; lemon</v>
+        <v>Gin or vodka with dry vermouth</v>
       </c>
       <c r="C41" t="str">
         <v>450</v>
@@ -1356,10 +1356,10 @@
     </row>
     <row r="42">
       <c r="A42" t="str">
-        <v>Mai Tai</v>
+        <v>Margarita</v>
       </c>
       <c r="B42" t="str">
-        <v>Rum, pineapple, lime &amp; almond</v>
+        <v>Tequila, lime &amp; triple sec with a salted rim</v>
       </c>
       <c r="C42" t="str">
         <v>450</v>
@@ -1379,16 +1379,16 @@
     </row>
     <row r="43">
       <c r="A43" t="str">
-        <v>Summer's Clarity</v>
+        <v>Manhattan</v>
       </c>
       <c r="B43" t="str">
-        <v>White rum with clarified watermelon, basil &amp; sparkle</v>
+        <v>Whisky stirred with sweet vermouth &amp; bitters</v>
       </c>
       <c r="C43" t="str">
-        <v>595</v>
+        <v>450</v>
       </c>
       <c r="D43" t="str">
-        <v>signature-cocktails</v>
+        <v>classic-cocktails</v>
       </c>
       <c r="E43" t="b">
         <v>1</v>
@@ -1402,16 +1402,16 @@
     </row>
     <row r="44">
       <c r="A44" t="str">
-        <v>Azure Bloom</v>
+        <v>Old Fashioned</v>
       </c>
       <c r="B44" t="str">
-        <v>Vodka, butterfly pea tea, mint &amp; airy carrot foam</v>
+        <v>Whisky, bitter &amp; sugar, stirred on ice</v>
       </c>
       <c r="C44" t="str">
-        <v>595</v>
+        <v>450</v>
       </c>
       <c r="D44" t="str">
-        <v>signature-cocktails</v>
+        <v>classic-cocktails</v>
       </c>
       <c r="E44" t="b">
         <v>1</v>
@@ -1425,10 +1425,10 @@
     </row>
     <row r="45">
       <c r="A45" t="str">
-        <v>The Gilded Fig</v>
+        <v>Summer's Clarity</v>
       </c>
       <c r="B45" t="str">
-        <v>Brandy with aromatic wine reduction &amp; fig syrup</v>
+        <v>White rum with clarified watermelon, basil &amp; sparkle</v>
       </c>
       <c r="C45" t="str">
         <v>595</v>
@@ -1448,10 +1448,10 @@
     </row>
     <row r="46">
       <c r="A46" t="str">
-        <v>The Mathri Merchant</v>
+        <v>Azure Bloom</v>
       </c>
       <c r="B46" t="str">
-        <v>Whisky, orange bitters, spiced syrup &amp; tea decoction</v>
+        <v>Vodka, butterfly pea tea, mint &amp; airy carrot foam</v>
       </c>
       <c r="C46" t="str">
         <v>595</v>
@@ -1471,10 +1471,10 @@
     </row>
     <row r="47">
       <c r="A47" t="str">
-        <v>The Tangent Trail</v>
+        <v>The Mathri Merchant</v>
       </c>
       <c r="B47" t="str">
-        <v>Tequila, spiced yuzu, pineapple &amp; milk clarification</v>
+        <v>Whisky, orange bitters, spiced syrup &amp; tea decoction</v>
       </c>
       <c r="C47" t="str">
         <v>595</v>
@@ -1540,16 +1540,16 @@
     </row>
     <row r="50">
       <c r="A50" t="str">
-        <v>Indigo Bloom</v>
+        <v>French 75</v>
       </c>
       <c r="B50" t="str">
-        <v>Gin, butterfly pea tea, elderflower &amp; tonic</v>
+        <v>Gin, lemon &amp; sparkling wine</v>
       </c>
       <c r="C50" t="str">
-        <v>595</v>
+        <v>375</v>
       </c>
       <c r="D50" t="str">
-        <v>signature-cocktails</v>
+        <v>wine-cocktails</v>
       </c>
       <c r="E50" t="b">
         <v>1</v>
@@ -1563,16 +1563,16 @@
     </row>
     <row r="51">
       <c r="A51" t="str">
-        <v>The Crimson Glass</v>
+        <v>Mimosa</v>
       </c>
       <c r="B51" t="str">
-        <v>Gin, cranberry, hibiscus &amp; milk clarity</v>
+        <v>Orange juice topped with sparkling wine</v>
       </c>
       <c r="C51" t="str">
-        <v>595</v>
+        <v>375</v>
       </c>
       <c r="D51" t="str">
-        <v>signature-cocktails</v>
+        <v>wine-cocktails</v>
       </c>
       <c r="E51" t="b">
         <v>1</v>
@@ -1586,16 +1586,16 @@
     </row>
     <row r="52">
       <c r="A52" t="str">
-        <v>Black Sands Swizzle</v>
+        <v>Bellini</v>
       </c>
       <c r="B52" t="str">
-        <v>White rum, charcoal, chilli bitters &amp; pineapple</v>
+        <v>Peach puree &amp; sparkling wine</v>
       </c>
       <c r="C52" t="str">
-        <v>595</v>
+        <v>375</v>
       </c>
       <c r="D52" t="str">
-        <v>signature-cocktails</v>
+        <v>wine-cocktails</v>
       </c>
       <c r="E52" t="b">
         <v>1</v>
@@ -1609,16 +1609,16 @@
     </row>
     <row r="53">
       <c r="A53" t="str">
-        <v>The Garden Fizz</v>
+        <v>Spritzer</v>
       </c>
       <c r="B53" t="str">
-        <v>Vodka, vanilla, basil, sweet &amp; sour &amp; ginger ale</v>
+        <v>White wine with soda</v>
       </c>
       <c r="C53" t="str">
-        <v>595</v>
+        <v>375</v>
       </c>
       <c r="D53" t="str">
-        <v>signature-cocktails</v>
+        <v>wine-cocktails</v>
       </c>
       <c r="E53" t="b">
         <v>1</v>
@@ -1632,16 +1632,16 @@
     </row>
     <row r="54">
       <c r="A54" t="str">
-        <v>The Midnight Affogato</v>
+        <v>Red Sangria</v>
       </c>
       <c r="B54" t="str">
-        <v>Vodka, vanilla, coffee &amp; cream</v>
+        <v>Red wine, citrus fruits &amp; spices</v>
       </c>
       <c r="C54" t="str">
-        <v>595</v>
+        <v>275 / 1200</v>
       </c>
       <c r="D54" t="str">
-        <v>signature-cocktails</v>
+        <v>sangria</v>
       </c>
       <c r="E54" t="b">
         <v>1</v>
@@ -1655,16 +1655,16 @@
     </row>
     <row r="55">
       <c r="A55" t="str">
-        <v>Barrel Bucket</v>
+        <v>White Sangria</v>
       </c>
       <c r="B55" t="str">
-        <v>Shareable, fun &amp; flavorful wine cocktails</v>
+        <v>White wine with tropical fruits</v>
       </c>
       <c r="C55" t="str">
-        <v>900</v>
+        <v>275 / 1200</v>
       </c>
       <c r="D55" t="str">
-        <v>signature-cocktails</v>
+        <v>sangria</v>
       </c>
       <c r="E55" t="b">
         <v>1</v>
@@ -1678,16 +1678,16 @@
     </row>
     <row r="56">
       <c r="A56" t="str">
-        <v>French 75</v>
+        <v>7 Spirits Sangria</v>
       </c>
       <c r="B56" t="str">
-        <v>Gin, lemon &amp; sparkling wine</v>
+        <v>A powerful mix of wine &amp; four white spirits</v>
       </c>
       <c r="C56" t="str">
-        <v>375</v>
+        <v>425 / 1700</v>
       </c>
       <c r="D56" t="str">
-        <v>wine-cocktails</v>
+        <v>sangria</v>
       </c>
       <c r="E56" t="b">
         <v>1</v>
@@ -1701,16 +1701,16 @@
     </row>
     <row r="57">
       <c r="A57" t="str">
-        <v>Mimosa</v>
+        <v>Kamikaze</v>
       </c>
       <c r="B57" t="str">
-        <v>Orange juice topped with sparkling wine</v>
+        <v>Signature shot</v>
       </c>
       <c r="C57" t="str">
-        <v>375</v>
+        <v>350 | Six: 1750</v>
       </c>
       <c r="D57" t="str">
-        <v>wine-cocktails</v>
+        <v>signature-shots</v>
       </c>
       <c r="E57" t="b">
         <v>1</v>
@@ -1724,16 +1724,16 @@
     </row>
     <row r="58">
       <c r="A58" t="str">
-        <v>Spritzer</v>
+        <v>B52</v>
       </c>
       <c r="B58" t="str">
-        <v>White wine with soda</v>
+        <v>Signature shot</v>
       </c>
       <c r="C58" t="str">
-        <v>375</v>
+        <v>400 | Six: 2000</v>
       </c>
       <c r="D58" t="str">
-        <v>wine-cocktails</v>
+        <v>signature-shots</v>
       </c>
       <c r="E58" t="b">
         <v>1</v>
@@ -1747,16 +1747,16 @@
     </row>
     <row r="59">
       <c r="A59" t="str">
-        <v>Bellini</v>
+        <v>Jägerbomb</v>
       </c>
       <c r="B59" t="str">
-        <v>Peach puree &amp; sparkling wine</v>
+        <v>Signature shot</v>
       </c>
       <c r="C59" t="str">
-        <v>375</v>
+        <v>450 | Six: 2250</v>
       </c>
       <c r="D59" t="str">
-        <v>wine-cocktails</v>
+        <v>signature-shots</v>
       </c>
       <c r="E59" t="b">
         <v>1</v>
@@ -1770,16 +1770,16 @@
     </row>
     <row r="60">
       <c r="A60" t="str">
-        <v>Marilyn Monroe</v>
+        <v>Flaming Lamborghini</v>
       </c>
       <c r="B60" t="str">
-        <v>A glamorous sparkling wine cocktail with fruity notes</v>
+        <v>Signature shot</v>
       </c>
       <c r="C60" t="str">
-        <v>375</v>
+        <v>2000</v>
       </c>
       <c r="D60" t="str">
-        <v>wine-cocktails</v>
+        <v>signature-shots</v>
       </c>
       <c r="E60" t="b">
         <v>1</v>
@@ -1793,16 +1793,16 @@
     </row>
     <row r="61">
       <c r="A61" t="str">
-        <v>Red Sangria</v>
+        <v>Johnnie Walker Black Label</v>
       </c>
       <c r="B61" t="str">
-        <v>Red wine, citrus fruits &amp; spices</v>
+        <v>Premium blended Scotch whisky</v>
       </c>
       <c r="C61" t="str">
-        <v>275 / 1200</v>
+        <v>850</v>
       </c>
       <c r="D61" t="str">
-        <v>sangria</v>
+        <v>blended-whisky</v>
       </c>
       <c r="E61" t="b">
         <v>1</v>
@@ -1816,16 +1816,16 @@
     </row>
     <row r="62">
       <c r="A62" t="str">
-        <v>White Sangria</v>
+        <v>Chivas Regal 12 Years</v>
       </c>
       <c r="B62" t="str">
-        <v>White wine with tropical fruits</v>
+        <v>Smooth blended Scotch whisky</v>
       </c>
       <c r="C62" t="str">
-        <v>275 / 1200</v>
+        <v>900</v>
       </c>
       <c r="D62" t="str">
-        <v>sangria</v>
+        <v>blended-whisky</v>
       </c>
       <c r="E62" t="b">
         <v>1</v>
@@ -1839,16 +1839,16 @@
     </row>
     <row r="63">
       <c r="A63" t="str">
-        <v>7 Spirits Sangria</v>
+        <v>Glenmorangie Original</v>
       </c>
       <c r="B63" t="str">
-        <v>A powerful mix of wine &amp; four white spirits</v>
+        <v>Single malt Scotch whisky</v>
       </c>
       <c r="C63" t="str">
-        <v>425 / 1700</v>
+        <v>950</v>
       </c>
       <c r="D63" t="str">
-        <v>sangria</v>
+        <v>single-malt-whisky</v>
       </c>
       <c r="E63" t="b">
         <v>1</v>
@@ -1862,16 +1862,16 @@
     </row>
     <row r="64">
       <c r="A64" t="str">
-        <v>Double Bubble</v>
+        <v>Macallan 12 Years</v>
       </c>
       <c r="B64" t="str">
-        <v>Sparkling wine + fruity sangria blend</v>
+        <v>Premium single malt whisky</v>
       </c>
       <c r="C64" t="str">
-        <v>425 / 1700</v>
+        <v>1200</v>
       </c>
       <c r="D64" t="str">
-        <v>sangria</v>
+        <v>single-malt-whisky</v>
       </c>
       <c r="E64" t="b">
         <v>1</v>
@@ -1885,16 +1885,16 @@
     </row>
     <row r="65">
       <c r="A65" t="str">
-        <v>Kamikaze</v>
+        <v>Balvenie DoubleWood</v>
       </c>
       <c r="B65" t="str">
-        <v>Signature shot</v>
+        <v>Rich single malt Scotch whisky</v>
       </c>
       <c r="C65" t="str">
-        <v>350 | Six: 1750</v>
+        <v>1100</v>
       </c>
       <c r="D65" t="str">
-        <v>signature-shots</v>
+        <v>single-malt-whisky</v>
       </c>
       <c r="E65" t="b">
         <v>1</v>
@@ -1908,16 +1908,16 @@
     </row>
     <row r="66">
       <c r="A66" t="str">
-        <v>B52</v>
+        <v>Jackass Broadside</v>
       </c>
       <c r="B66" t="str">
-        <v>Signature shot</v>
+        <v>American Irish whiskey</v>
       </c>
       <c r="C66" t="str">
-        <v>400 | Six: 2000</v>
+        <v>850</v>
       </c>
       <c r="D66" t="str">
-        <v>signature-shots</v>
+        <v>american-irish-whiskey</v>
       </c>
       <c r="E66" t="b">
         <v>1</v>
@@ -1931,16 +1931,16 @@
     </row>
     <row r="67">
       <c r="A67" t="str">
-        <v>Jägerbomb</v>
+        <v>Blended Scotch Whisky</v>
       </c>
       <c r="B67" t="str">
-        <v>Signature shot</v>
+        <v>Classic blended whisky</v>
       </c>
       <c r="C67" t="str">
-        <v>450 | Six: 2250</v>
+        <v>750</v>
       </c>
       <c r="D67" t="str">
-        <v>signature-shots</v>
+        <v>blended-scotch-whisky</v>
       </c>
       <c r="E67" t="b">
         <v>1</v>
@@ -1954,16 +1954,16 @@
     </row>
     <row r="68">
       <c r="A68" t="str">
-        <v>Mini Jägerbomb</v>
+        <v>Absolut Vodka</v>
       </c>
       <c r="B68" t="str">
-        <v>Mini Jägerbomb (10 for 5)</v>
+        <v>Premium Swedish vodka</v>
       </c>
       <c r="C68" t="str">
-        <v>1000 | 5000</v>
+        <v>750</v>
       </c>
       <c r="D68" t="str">
-        <v>signature-shots</v>
+        <v>vodka</v>
       </c>
       <c r="E68" t="b">
         <v>1</v>
@@ -1977,16 +1977,16 @@
     </row>
     <row r="69">
       <c r="A69" t="str">
-        <v>Lemon Drop</v>
+        <v>Tanqueray Gin</v>
       </c>
       <c r="B69" t="str">
-        <v>Signature shot</v>
+        <v>Classic London dry gin</v>
       </c>
       <c r="C69" t="str">
-        <v>350 | Six: 1750</v>
+        <v>850</v>
       </c>
       <c r="D69" t="str">
-        <v>signature-shots</v>
+        <v>gin</v>
       </c>
       <c r="E69" t="b">
         <v>1</v>
@@ -2000,16 +2000,16 @@
     </row>
     <row r="70">
       <c r="A70" t="str">
-        <v>Monk Chocolate</v>
+        <v>Bacardi Rum</v>
       </c>
       <c r="B70" t="str">
-        <v>Signature shot</v>
+        <v>Light premium rum</v>
       </c>
       <c r="C70" t="str">
-        <v>350 | Six: 1750</v>
+        <v>700</v>
       </c>
       <c r="D70" t="str">
-        <v>signature-shots</v>
+        <v>rum</v>
       </c>
       <c r="E70" t="b">
         <v>1</v>
@@ -2023,16 +2023,16 @@
     </row>
     <row r="71">
       <c r="A71" t="str">
-        <v>Flaming Lamborghini</v>
+        <v>Jose Cuervo Tequila</v>
       </c>
       <c r="B71" t="str">
-        <v>Signature shot</v>
+        <v>Traditional tequila</v>
       </c>
       <c r="C71" t="str">
-        <v>2000</v>
+        <v>800</v>
       </c>
       <c r="D71" t="str">
-        <v>signature-shots</v>
+        <v>tequila</v>
       </c>
       <c r="E71" t="b">
         <v>1</v>
@@ -2046,16 +2046,16 @@
     </row>
     <row r="72">
       <c r="A72" t="str">
-        <v>Fire Shot</v>
+        <v>Hennessy Cognac</v>
       </c>
       <c r="B72" t="str">
-        <v>Signature shot</v>
+        <v>Premium French cognac</v>
       </c>
       <c r="C72" t="str">
-        <v>400 | Six: 2000</v>
+        <v>1500</v>
       </c>
       <c r="D72" t="str">
-        <v>signature-shots</v>
+        <v>cognac-brandy</v>
       </c>
       <c r="E72" t="b">
         <v>1</v>
@@ -2064,12 +2064,472 @@
         <v/>
       </c>
       <c r="G72" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="str">
+        <v>Cointreau Liqueur</v>
+      </c>
+      <c r="B73" t="str">
+        <v>Premium triple sec liqueur</v>
+      </c>
+      <c r="C73" t="str">
+        <v>900</v>
+      </c>
+      <c r="D73" t="str">
+        <v>liqueurs</v>
+      </c>
+      <c r="E73" t="b">
+        <v>1</v>
+      </c>
+      <c r="F73" t="str">
+        <v/>
+      </c>
+      <c r="G73" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="str">
+        <v>Perrier-Jouet Champagne</v>
+      </c>
+      <c r="B74" t="str">
+        <v>Premium sparkling wine</v>
+      </c>
+      <c r="C74" t="str">
+        <v>2500</v>
+      </c>
+      <c r="D74" t="str">
+        <v>sparkling-wine</v>
+      </c>
+      <c r="E74" t="b">
+        <v>1</v>
+      </c>
+      <c r="F74" t="str">
+        <v/>
+      </c>
+      <c r="G74" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="str">
+        <v>Barefoot Sauvignon Blanc</v>
+      </c>
+      <c r="B75" t="str">
+        <v>Crisp white wine from California</v>
+      </c>
+      <c r="C75" t="str">
+        <v>1200</v>
+      </c>
+      <c r="D75" t="str">
+        <v>white-wines</v>
+      </c>
+      <c r="E75" t="b">
+        <v>1</v>
+      </c>
+      <c r="F75" t="str">
+        <v/>
+      </c>
+      <c r="G75" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="str">
+        <v>La Crema Chardonnay</v>
+      </c>
+      <c r="B76" t="str">
+        <v>Full-bodied white wine</v>
+      </c>
+      <c r="C76" t="str">
+        <v>1400</v>
+      </c>
+      <c r="D76" t="str">
+        <v>white-wines</v>
+      </c>
+      <c r="E76" t="b">
+        <v>1</v>
+      </c>
+      <c r="F76" t="str">
+        <v/>
+      </c>
+      <c r="G76" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="str">
+        <v>Sutter Home White Zinfandel</v>
+      </c>
+      <c r="B77" t="str">
+        <v>Sweet rose wine</v>
+      </c>
+      <c r="C77" t="str">
+        <v>1100</v>
+      </c>
+      <c r="D77" t="str">
+        <v>rose-wines</v>
+      </c>
+      <c r="E77" t="b">
+        <v>1</v>
+      </c>
+      <c r="F77" t="str">
+        <v/>
+      </c>
+      <c r="G77" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="str">
+        <v>Yellow Tail Cabernet Sauvignon</v>
+      </c>
+      <c r="B78" t="str">
+        <v>Rich red wine from Australia</v>
+      </c>
+      <c r="C78" t="str">
+        <v>1300</v>
+      </c>
+      <c r="D78" t="str">
+        <v>red-wines</v>
+      </c>
+      <c r="E78" t="b">
+        <v>1</v>
+      </c>
+      <c r="F78" t="str">
+        <v/>
+      </c>
+      <c r="G78" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="str">
+        <v>Barefoot Pinot Noir</v>
+      </c>
+      <c r="B79" t="str">
+        <v>Smooth red wine</v>
+      </c>
+      <c r="C79" t="str">
+        <v>1250</v>
+      </c>
+      <c r="D79" t="str">
+        <v>red-wines</v>
+      </c>
+      <c r="E79" t="b">
+        <v>1</v>
+      </c>
+      <c r="F79" t="str">
+        <v/>
+      </c>
+      <c r="G79" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="str">
+        <v>Bota Box Pinot Grigio</v>
+      </c>
+      <c r="B80" t="str">
+        <v>Affordable white wine box</v>
+      </c>
+      <c r="C80" t="str">
+        <v>950</v>
+      </c>
+      <c r="D80" t="str">
+        <v>white-wines</v>
+      </c>
+      <c r="E80" t="b">
+        <v>1</v>
+      </c>
+      <c r="F80" t="str">
+        <v/>
+      </c>
+      <c r="G80" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="str">
+        <v>Barefoot Red Blend</v>
+      </c>
+      <c r="B81" t="str">
+        <v>Fruit-forward red wine blend</v>
+      </c>
+      <c r="C81" t="str">
+        <v>1150</v>
+      </c>
+      <c r="D81" t="str">
+        <v>red-wines</v>
+      </c>
+      <c r="E81" t="b">
+        <v>1</v>
+      </c>
+      <c r="F81" t="str">
+        <v/>
+      </c>
+      <c r="G81" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="str">
+        <v>Barefoot Merlot</v>
+      </c>
+      <c r="B82" t="str">
+        <v>Smooth red wine</v>
+      </c>
+      <c r="C82" t="str">
+        <v>1200</v>
+      </c>
+      <c r="D82" t="str">
+        <v>red-wines</v>
+      </c>
+      <c r="E82" t="b">
+        <v>1</v>
+      </c>
+      <c r="F82" t="str">
+        <v/>
+      </c>
+      <c r="G82" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="str">
+        <v>Barefoot Cabernet Sauvignon</v>
+      </c>
+      <c r="B83" t="str">
+        <v>Bold red wine</v>
+      </c>
+      <c r="C83" t="str">
+        <v>1300</v>
+      </c>
+      <c r="D83" t="str">
+        <v>red-wines</v>
+      </c>
+      <c r="E83" t="b">
+        <v>1</v>
+      </c>
+      <c r="F83" t="str">
+        <v/>
+      </c>
+      <c r="G83" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="str">
+        <v>Taylor Dessert Wine</v>
+      </c>
+      <c r="B84" t="str">
+        <v>Sweet dessert wine</v>
+      </c>
+      <c r="C84" t="str">
+        <v>1100</v>
+      </c>
+      <c r="D84" t="str">
+        <v>dessert-wines</v>
+      </c>
+      <c r="E84" t="b">
+        <v>1</v>
+      </c>
+      <c r="F84" t="str">
+        <v/>
+      </c>
+      <c r="G84" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="str">
+        <v>Barefoot Zinfandel</v>
+      </c>
+      <c r="B85" t="str">
+        <v>Rich dessert wine</v>
+      </c>
+      <c r="C85" t="str">
+        <v>1250</v>
+      </c>
+      <c r="D85" t="str">
+        <v>dessert-wines</v>
+      </c>
+      <c r="E85" t="b">
+        <v>1</v>
+      </c>
+      <c r="F85" t="str">
+        <v/>
+      </c>
+      <c r="G85" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="str">
+        <v>Sandeman Tawny Port</v>
+      </c>
+      <c r="B86" t="str">
+        <v>Classic tawny port wine</v>
+      </c>
+      <c r="C86" t="str">
+        <v>1400</v>
+      </c>
+      <c r="D86" t="str">
+        <v>port-wine</v>
+      </c>
+      <c r="E86" t="b">
+        <v>1</v>
+      </c>
+      <c r="F86" t="str">
+        <v/>
+      </c>
+      <c r="G86" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="str">
+        <v>Barefoot Riesling</v>
+      </c>
+      <c r="B87" t="str">
+        <v>Semi-sweet white wine</v>
+      </c>
+      <c r="C87" t="str">
+        <v>1150</v>
+      </c>
+      <c r="D87" t="str">
+        <v>dessert-wines</v>
+      </c>
+      <c r="E87" t="b">
+        <v>1</v>
+      </c>
+      <c r="F87" t="str">
+        <v/>
+      </c>
+      <c r="G87" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="str">
+        <v>Mojito Mocktail</v>
+      </c>
+      <c r="B88" t="str">
+        <v>Fresh mint &amp; lime mocktail</v>
+      </c>
+      <c r="C88" t="str">
+        <v>250</v>
+      </c>
+      <c r="D88" t="str">
+        <v>signature-mocktails</v>
+      </c>
+      <c r="E88" t="b">
+        <v>1</v>
+      </c>
+      <c r="F88" t="str">
+        <v/>
+      </c>
+      <c r="G88" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="str">
+        <v>Virgin Margarita</v>
+      </c>
+      <c r="B89" t="str">
+        <v>Refreshing margarita without alcohol</v>
+      </c>
+      <c r="C89" t="str">
+        <v>250</v>
+      </c>
+      <c r="D89" t="str">
+        <v>signature-mocktails</v>
+      </c>
+      <c r="E89" t="b">
+        <v>1</v>
+      </c>
+      <c r="F89" t="str">
+        <v/>
+      </c>
+      <c r="G89" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="str">
+        <v>Lemonade</v>
+      </c>
+      <c r="B90" t="str">
+        <v>Fresh homemade lemonade</v>
+      </c>
+      <c r="C90" t="str">
+        <v>150</v>
+      </c>
+      <c r="D90" t="str">
+        <v>soft-beverages</v>
+      </c>
+      <c r="E90" t="b">
+        <v>1</v>
+      </c>
+      <c r="F90" t="str">
+        <v/>
+      </c>
+      <c r="G90" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="str">
+        <v>Iced Tea</v>
+      </c>
+      <c r="B91" t="str">
+        <v>Chilled iced tea</v>
+      </c>
+      <c r="C91" t="str">
+        <v>120</v>
+      </c>
+      <c r="D91" t="str">
+        <v>soft-beverages</v>
+      </c>
+      <c r="E91" t="b">
+        <v>1</v>
+      </c>
+      <c r="F91" t="str">
+        <v/>
+      </c>
+      <c r="G91" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="str">
+        <v>Mango Lassi</v>
+      </c>
+      <c r="B92" t="str">
+        <v>Traditional yogurt-based mango drink</v>
+      </c>
+      <c r="C92" t="str">
+        <v>180</v>
+      </c>
+      <c r="D92" t="str">
+        <v>soft-beverages</v>
+      </c>
+      <c r="E92" t="b">
+        <v>1</v>
+      </c>
+      <c r="F92" t="str">
+        <v/>
+      </c>
+      <c r="G92" t="b">
         <v>1</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:G72"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:G92"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Create Excel file with only beverage and cocktail menu items
Generate BarrelBorn_Menu_Template.xlsx containing 71 items across categories like Craft Beers, Draught Beer, Pint Beers, Classic Cocktails, Signature Cocktails, Wine Cocktails, Sangria, and Signature Shots.

Replit-Commit-Author: Agent
Replit-Commit-Session-Id: d5825b2d-5a70-4950-bc3e-e69072dc9210
Replit-Commit-Checkpoint-Type: full_checkpoint
Replit-Commit-Event-Id: 78d37ec6-ca5f-498f-938a-54e986d2ecc0
Replit-Commit-Screenshot-Url: https://storage.googleapis.com/screenshot-production-us-central1/a0e76cf1-50a4-4033-88e9-413827fbeca2/d5825b2d-5a70-4950-bc3e-e69072dc9210/hllg6Je
Replit-Helium-Checkpoint-Created: true
</commit_message>
<xml_diff>
--- a/BarrelBorn_Menu_Template.xlsx
+++ b/BarrelBorn_Menu_Template.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G92"/>
+  <dimension ref="A1:G72"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -436,16 +436,16 @@
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>Samosa (2 pcs)</v>
+        <v>Gateway White Zen</v>
       </c>
       <c r="B2" t="str">
-        <v>Crispy potato &amp; pea pastry</v>
+        <v>Light German Style Wheat Beer</v>
       </c>
       <c r="C2" t="str">
-        <v>120</v>
+        <v>265 / 485 / 1350</v>
       </c>
       <c r="D2" t="str">
-        <v>nibbles</v>
+        <v>craft-beers-on-tap</v>
       </c>
       <c r="E2" t="b">
         <v>1</v>
@@ -459,16 +459,16 @@
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v>Paneer Tikka Masala</v>
+        <v>Gateway Doppelganger</v>
       </c>
       <c r="B3" t="str">
-        <v>Cottage cheese cubes in creamy tomato gravy</v>
+        <v>Smooth German-style Coffee Stout</v>
       </c>
       <c r="C3" t="str">
-        <v>249</v>
+        <v>265 / 485 / 1350</v>
       </c>
       <c r="D3" t="str">
-        <v>starters</v>
+        <v>craft-beers-on-tap</v>
       </c>
       <c r="E3" t="b">
         <v>1</v>
@@ -482,19 +482,19 @@
     </row>
     <row r="4">
       <c r="A4" t="str">
-        <v>Chicken Biryani</v>
+        <v>Bira 91 Pilsner</v>
       </c>
       <c r="B4" t="str">
-        <v>Aromatic basmati rice cooked with tender chicken</v>
+        <v>Crisp, refreshing, easy-drinking</v>
       </c>
       <c r="C4" t="str">
-        <v>299</v>
+        <v>235 / 410 / 1195</v>
       </c>
       <c r="D4" t="str">
-        <v>biryani</v>
+        <v>craft-beers-on-tap</v>
       </c>
       <c r="E4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F4" t="str">
         <v/>
@@ -505,16 +505,16 @@
     </row>
     <row r="5">
       <c r="A5" t="str">
-        <v>Paneer Butter Masala</v>
+        <v>Bira 91 Belgian Golden Strong Ale</v>
       </c>
       <c r="B5" t="str">
-        <v>Soft paneer cubes in rich butter sauce</v>
+        <v>Fruity, Belgian-style</v>
       </c>
       <c r="C5" t="str">
-        <v>249</v>
+        <v>235 / 410 / 1195</v>
       </c>
       <c r="D5" t="str">
-        <v>entree</v>
+        <v>craft-beers-on-tap</v>
       </c>
       <c r="E5" t="b">
         <v>1</v>
@@ -528,19 +528,19 @@
     </row>
     <row r="6">
       <c r="A6" t="str">
-        <v>Butter Chicken</v>
+        <v>Bira 91 WC IPA</v>
       </c>
       <c r="B6" t="str">
-        <v>Tender chicken in creamy tomato sauce</v>
+        <v>Hoppy, bold &amp; aromatic</v>
       </c>
       <c r="C6" t="str">
-        <v>279</v>
+        <v>235 / 410 / 1195</v>
       </c>
       <c r="D6" t="str">
-        <v>entree</v>
+        <v>craft-beers-on-tap</v>
       </c>
       <c r="E6" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F6" t="str">
         <v/>
@@ -551,16 +551,16 @@
     </row>
     <row r="7">
       <c r="A7" t="str">
-        <v>Butter Naan</v>
+        <v>Bira 91 Hefeweizen</v>
       </c>
       <c r="B7" t="str">
-        <v>Soft Indian bread brushed with butter</v>
+        <v>Smooth wheat beer with banana &amp; clove notes</v>
       </c>
       <c r="C7" t="str">
-        <v>80</v>
+        <v>235 / 410 / 1195</v>
       </c>
       <c r="D7" t="str">
-        <v>breads</v>
+        <v>craft-beers-on-tap</v>
       </c>
       <c r="E7" t="b">
         <v>1</v>
@@ -574,16 +574,16 @@
     </row>
     <row r="8">
       <c r="A8" t="str">
-        <v>Garlic Naan</v>
+        <v>Drifter Basmati</v>
       </c>
       <c r="B8" t="str">
-        <v>Naan topped with garlic &amp; herbs</v>
+        <v>Unique basmati aroma, super smooth</v>
       </c>
       <c r="C8" t="str">
-        <v>90</v>
+        <v>245 / 460 / 1330</v>
       </c>
       <c r="D8" t="str">
-        <v>breads</v>
+        <v>craft-beers-on-tap</v>
       </c>
       <c r="E8" t="b">
         <v>1</v>
@@ -597,16 +597,16 @@
     </row>
     <row r="9">
       <c r="A9" t="str">
-        <v>Dal Makhani</v>
+        <v>Drifter Cream Stout</v>
       </c>
       <c r="B9" t="str">
-        <v>Creamy black lentil preparation</v>
+        <v>Dark, creamy, chocolate &amp; coffee notes</v>
       </c>
       <c r="C9" t="str">
-        <v>199</v>
+        <v>245 / 460 / 1330</v>
       </c>
       <c r="D9" t="str">
-        <v>dals</v>
+        <v>craft-beers-on-tap</v>
       </c>
       <c r="E9" t="b">
         <v>1</v>
@@ -620,19 +620,19 @@
     </row>
     <row r="10">
       <c r="A10" t="str">
-        <v>Tandoori Chicken</v>
+        <v>Drifter Kokam Cider</v>
       </c>
       <c r="B10" t="str">
-        <v>Grilled chicken marinated in yogurt &amp; spices</v>
+        <v>Tart, fruity cider with coastal kokam</v>
       </c>
       <c r="C10" t="str">
-        <v>249</v>
+        <v>245 / 460 / 1330</v>
       </c>
       <c r="D10" t="str">
-        <v>charcoal</v>
+        <v>craft-beers-on-tap</v>
       </c>
       <c r="E10" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F10" t="str">
         <v/>
@@ -643,16 +643,16 @@
     </row>
     <row r="11">
       <c r="A11" t="str">
-        <v>Paneer Tikka</v>
+        <v>Kingfisher Draught</v>
       </c>
       <c r="B11" t="str">
-        <v>Marinated paneer grilled in tandoor</v>
+        <v>Classic, smooth, perfect for sessions</v>
       </c>
       <c r="C11" t="str">
-        <v>219</v>
+        <v>255 / 375 / 995</v>
       </c>
       <c r="D11" t="str">
-        <v>charcoal</v>
+        <v>draught-beer</v>
       </c>
       <c r="E11" t="b">
         <v>1</v>
@@ -666,19 +666,19 @@
     </row>
     <row r="12">
       <c r="A12" t="str">
-        <v>Pasta Carbonara</v>
+        <v>Hoegaarden</v>
       </c>
       <c r="B12" t="str">
-        <v>Creamy pasta with bacon &amp; parmesan</v>
+        <v>Belgian wheat beer – smooth &amp; citrusy</v>
       </c>
       <c r="C12" t="str">
-        <v>249</v>
+        <v>495</v>
       </c>
       <c r="D12" t="str">
-        <v>pasta</v>
+        <v>pint-beers</v>
       </c>
       <c r="E12" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F12" t="str">
         <v/>
@@ -689,16 +689,16 @@
     </row>
     <row r="13">
       <c r="A13" t="str">
-        <v>Margherita Pizza</v>
+        <v>Corona</v>
       </c>
       <c r="B13" t="str">
-        <v>Fresh mozzarella, tomato &amp; basil on thin crust</v>
+        <v>Light &amp; crisp — best with lime</v>
       </c>
       <c r="C13" t="str">
-        <v>249</v>
+        <v>495</v>
       </c>
       <c r="D13" t="str">
-        <v>pizza</v>
+        <v>pint-beers</v>
       </c>
       <c r="E13" t="b">
         <v>1</v>
@@ -712,19 +712,19 @@
     </row>
     <row r="14">
       <c r="A14" t="str">
-        <v>Chicken Slider</v>
+        <v>Kingfisher Strong</v>
       </c>
       <c r="B14" t="str">
-        <v>Grilled chicken burger on soft roll</v>
+        <v>Strong &amp; popular lager</v>
       </c>
       <c r="C14" t="str">
-        <v>149</v>
+        <v>375</v>
       </c>
       <c r="D14" t="str">
-        <v>sliders</v>
+        <v>pint-beers</v>
       </c>
       <c r="E14" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F14" t="str">
         <v/>
@@ -735,19 +735,19 @@
     </row>
     <row r="15">
       <c r="A15" t="str">
-        <v>Thai Green Curry</v>
+        <v>Budweiser Magnum</v>
       </c>
       <c r="B15" t="str">
-        <v>Aromatic green curry with chicken &amp; vegetables</v>
+        <v>Strong &amp; popular lager</v>
       </c>
       <c r="C15" t="str">
-        <v>279</v>
+        <v>435</v>
       </c>
       <c r="D15" t="str">
-        <v>thai-bowls</v>
+        <v>pint-beers</v>
       </c>
       <c r="E15" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F15" t="str">
         <v/>
@@ -758,19 +758,19 @@
     </row>
     <row r="16">
       <c r="A16" t="str">
-        <v>Rice Noodles with Shrimp</v>
+        <v>Carlsberg Elephant</v>
       </c>
       <c r="B16" t="str">
-        <v>Stir-fried rice noodles with fresh shrimp</v>
+        <v>Strong &amp; popular lager</v>
       </c>
       <c r="C16" t="str">
-        <v>299</v>
+        <v>375</v>
       </c>
       <c r="D16" t="str">
-        <v>rice-noodles</v>
+        <v>pint-beers</v>
       </c>
       <c r="E16" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F16" t="str">
         <v/>
@@ -781,16 +781,16 @@
     </row>
     <row r="17">
       <c r="A17" t="str">
-        <v>Vegetable Sizzler</v>
+        <v>Budweiser</v>
       </c>
       <c r="B17" t="str">
-        <v>Grilled seasonal vegetables on hot plate</v>
+        <v>Easy drinking lager</v>
       </c>
       <c r="C17" t="str">
-        <v>249</v>
+        <v>345</v>
       </c>
       <c r="D17" t="str">
-        <v>sizzlers</v>
+        <v>pint-beers</v>
       </c>
       <c r="E17" t="b">
         <v>1</v>
@@ -804,19 +804,19 @@
     </row>
     <row r="18">
       <c r="A18" t="str">
-        <v>Chicken Sizzler</v>
+        <v>Amstel Light</v>
       </c>
       <c r="B18" t="str">
-        <v>Grilled chicken strips on hot plate</v>
+        <v>Easy drinking lager</v>
       </c>
       <c r="C18" t="str">
-        <v>349</v>
+        <v>375</v>
       </c>
       <c r="D18" t="str">
-        <v>sizzlers</v>
+        <v>pint-beers</v>
       </c>
       <c r="E18" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F18" t="str">
         <v/>
@@ -827,19 +827,19 @@
     </row>
     <row r="19">
       <c r="A19" t="str">
-        <v>Dim Sum Platter</v>
+        <v>Carlsberg Smooth</v>
       </c>
       <c r="B19" t="str">
-        <v>Assorted steamed dumplings with dipping sauces</v>
+        <v>Easy drinking lager</v>
       </c>
       <c r="C19" t="str">
-        <v>299</v>
+        <v>345</v>
       </c>
       <c r="D19" t="str">
-        <v>bao-dimsum</v>
+        <v>pint-beers</v>
       </c>
       <c r="E19" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F19" t="str">
         <v/>
@@ -850,16 +850,16 @@
     </row>
     <row r="20">
       <c r="A20" t="str">
-        <v>Paneer Curry</v>
+        <v>Heineken</v>
       </c>
       <c r="B20" t="str">
-        <v>Paneer in aromatic curry sauce</v>
+        <v>Easy drinking lager</v>
       </c>
       <c r="C20" t="str">
-        <v>229</v>
+        <v>345</v>
       </c>
       <c r="D20" t="str">
-        <v>curries</v>
+        <v>pint-beers</v>
       </c>
       <c r="E20" t="b">
         <v>1</v>
@@ -873,19 +873,19 @@
     </row>
     <row r="21">
       <c r="A21" t="str">
-        <v>Chicken Curry</v>
+        <v>KF Mild</v>
       </c>
       <c r="B21" t="str">
-        <v>Tender chicken in rich gravy</v>
+        <v>Value friendly pick</v>
       </c>
       <c r="C21" t="str">
-        <v>249</v>
+        <v>275</v>
       </c>
       <c r="D21" t="str">
-        <v>curries</v>
+        <v>pint-beers</v>
       </c>
       <c r="E21" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F21" t="str">
         <v/>
@@ -896,16 +896,16 @@
     </row>
     <row r="22">
       <c r="A22" t="str">
-        <v>Vegetable Biryani</v>
+        <v>KF Ultra</v>
       </c>
       <c r="B22" t="str">
-        <v>Aromatic rice with mixed vegetables</v>
+        <v>Value friendly pick</v>
       </c>
       <c r="C22" t="str">
-        <v>229</v>
+        <v>325</v>
       </c>
       <c r="D22" t="str">
-        <v>biryani</v>
+        <v>pint-beers</v>
       </c>
       <c r="E22" t="b">
         <v>1</v>
@@ -919,16 +919,16 @@
     </row>
     <row r="23">
       <c r="A23" t="str">
-        <v>Lentil Soup</v>
+        <v>Tuborg Green</v>
       </c>
       <c r="B23" t="str">
-        <v>Creamy lentil &amp; vegetable soup</v>
+        <v>Value friendly pick</v>
       </c>
       <c r="C23" t="str">
-        <v>149</v>
+        <v>325</v>
       </c>
       <c r="D23" t="str">
-        <v>soups</v>
+        <v>pint-beers</v>
       </c>
       <c r="E23" t="b">
         <v>1</v>
@@ -942,19 +942,19 @@
     </row>
     <row r="24">
       <c r="A24" t="str">
-        <v>Chicken Soup</v>
+        <v>Tuborg</v>
       </c>
       <c r="B24" t="str">
-        <v>Light broth with chicken &amp; vegetables</v>
+        <v>Value friendly pick</v>
       </c>
       <c r="C24" t="str">
-        <v>169</v>
+        <v>325</v>
       </c>
       <c r="D24" t="str">
-        <v>soups</v>
+        <v>pint-beers</v>
       </c>
       <c r="E24" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F24" t="str">
         <v/>
@@ -965,16 +965,16 @@
     </row>
     <row r="25">
       <c r="A25" t="str">
-        <v>Rocket &amp; Parmesan Salad</v>
+        <v>Peoples Lager</v>
       </c>
       <c r="B25" t="str">
-        <v>Fresh arugula with shaved parmesan &amp; balsamic</v>
+        <v>Local craft-style lager</v>
       </c>
       <c r="C25" t="str">
-        <v>199</v>
+        <v>405</v>
       </c>
       <c r="D25" t="str">
-        <v>salads</v>
+        <v>pint-beers</v>
       </c>
       <c r="E25" t="b">
         <v>1</v>
@@ -988,19 +988,19 @@
     </row>
     <row r="26">
       <c r="A26" t="str">
-        <v>Grilled Chicken Salad</v>
+        <v>Breezer</v>
       </c>
       <c r="B26" t="str">
-        <v>Mixed greens with grilled chicken strips</v>
+        <v>Fruity, refreshing, low-alcohol</v>
       </c>
       <c r="C26" t="str">
-        <v>249</v>
+        <v>350</v>
       </c>
       <c r="D26" t="str">
-        <v>salads</v>
+        <v>pint-beers</v>
       </c>
       <c r="E26" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F26" t="str">
         <v/>
@@ -1011,19 +1011,19 @@
     </row>
     <row r="27">
       <c r="A27" t="str">
-        <v>Asian Noodles</v>
+        <v>LIIT</v>
       </c>
       <c r="B27" t="str">
-        <v>Stir-fried noodles with Asian flavors</v>
+        <v>Powerful blend of five white spirits, citrus, and cola. Our strongest classic.</v>
       </c>
       <c r="C27" t="str">
-        <v>229</v>
+        <v>800</v>
       </c>
       <c r="D27" t="str">
-        <v>asian-mains</v>
+        <v>classic-cocktails</v>
       </c>
       <c r="E27" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F27" t="str">
         <v/>
@@ -1034,16 +1034,16 @@
     </row>
     <row r="28">
       <c r="A28" t="str">
-        <v>Gateway White Zen</v>
+        <v>Mojito</v>
       </c>
       <c r="B28" t="str">
-        <v>Light German Style Wheat Beer</v>
+        <v>Fresh mint, lime, sugar, and white rum topped with soda. Crisp, refreshing, perfect anytime.</v>
       </c>
       <c r="C28" t="str">
-        <v>265 / 485 / 1350</v>
+        <v>450</v>
       </c>
       <c r="D28" t="str">
-        <v>craft-beers-on-tap</v>
+        <v>classic-cocktails</v>
       </c>
       <c r="E28" t="b">
         <v>1</v>
@@ -1057,16 +1057,16 @@
     </row>
     <row r="29">
       <c r="A29" t="str">
-        <v>Gateway Doppelganger</v>
+        <v>Martini</v>
       </c>
       <c r="B29" t="str">
-        <v>Smooth German-style Coffee Stout</v>
+        <v>The timeless mix of gin or vodka with dry vermouth. Elegantly stiff and refined.</v>
       </c>
       <c r="C29" t="str">
-        <v>265 / 485 / 1350</v>
+        <v>450</v>
       </c>
       <c r="D29" t="str">
-        <v>craft-beers-on-tap</v>
+        <v>classic-cocktails</v>
       </c>
       <c r="E29" t="b">
         <v>1</v>
@@ -1080,16 +1080,16 @@
     </row>
     <row r="30">
       <c r="A30" t="str">
-        <v>Bira 91 Pilsner</v>
+        <v>Manhattan</v>
       </c>
       <c r="B30" t="str">
-        <v>Crisp, refreshing, easy-drinking</v>
+        <v>Whisky stirred with sweet vermouth &amp; bitters. A smooth, mature classic.</v>
       </c>
       <c r="C30" t="str">
-        <v>235 / 410 / 1195</v>
+        <v>450</v>
       </c>
       <c r="D30" t="str">
-        <v>craft-beers-on-tap</v>
+        <v>classic-cocktails</v>
       </c>
       <c r="E30" t="b">
         <v>1</v>
@@ -1103,16 +1103,16 @@
     </row>
     <row r="31">
       <c r="A31" t="str">
-        <v>Bira 91 Belgian Golden Strong Ale</v>
+        <v>Cosmopolitan</v>
       </c>
       <c r="B31" t="str">
-        <v>Fruity, Belgian-style</v>
+        <v>Vodka, cranberry, lime &amp; triple sec. Vibrant, fruity &amp; stylish.</v>
       </c>
       <c r="C31" t="str">
-        <v>235 / 410 / 1195</v>
+        <v>450</v>
       </c>
       <c r="D31" t="str">
-        <v>craft-beers-on-tap</v>
+        <v>classic-cocktails</v>
       </c>
       <c r="E31" t="b">
         <v>1</v>
@@ -1126,16 +1126,16 @@
     </row>
     <row r="32">
       <c r="A32" t="str">
-        <v>Bira 91 WC IPA</v>
+        <v>Pina Colada</v>
       </c>
       <c r="B32" t="str">
-        <v>Hoppy, bold &amp; aromatic</v>
+        <v>Pineapple, coconut cream &amp; rum. A tropical holiday in a glass.</v>
       </c>
       <c r="C32" t="str">
-        <v>235 / 410 / 1195</v>
+        <v>450</v>
       </c>
       <c r="D32" t="str">
-        <v>craft-beers-on-tap</v>
+        <v>classic-cocktails</v>
       </c>
       <c r="E32" t="b">
         <v>1</v>
@@ -1149,16 +1149,16 @@
     </row>
     <row r="33">
       <c r="A33" t="str">
-        <v>Drifter Basmati</v>
+        <v>Margarita</v>
       </c>
       <c r="B33" t="str">
-        <v>Unique basmati aroma, super smooth</v>
+        <v>Tequila, lime &amp; triple sec with a salted rim. Zesty, bright &amp; perfectly balanced.</v>
       </c>
       <c r="C33" t="str">
-        <v>245 / 460 / 1330</v>
+        <v>450</v>
       </c>
       <c r="D33" t="str">
-        <v>craft-beers-on-tap</v>
+        <v>classic-cocktails</v>
       </c>
       <c r="E33" t="b">
         <v>1</v>
@@ -1172,16 +1172,16 @@
     </row>
     <row r="34">
       <c r="A34" t="str">
-        <v>Drifter Cream Stout</v>
+        <v>Moscow Mule</v>
       </c>
       <c r="B34" t="str">
-        <v>Dark, creamy, chocolate &amp; coffee notes</v>
+        <v>Vodka, ginger beer &amp; lime served cold. Bold, spicy &amp; refreshing.</v>
       </c>
       <c r="C34" t="str">
-        <v>245 / 460 / 1330</v>
+        <v>450</v>
       </c>
       <c r="D34" t="str">
-        <v>craft-beers-on-tap</v>
+        <v>classic-cocktails</v>
       </c>
       <c r="E34" t="b">
         <v>1</v>
@@ -1195,16 +1195,16 @@
     </row>
     <row r="35">
       <c r="A35" t="str">
-        <v>Kingfisher Draught</v>
+        <v>Old Fashioned</v>
       </c>
       <c r="B35" t="str">
-        <v>Classic, smooth, perfect for sessions</v>
+        <v>Whisky, bitter &amp; sugar, stirred on ice. A smooth, powerful gentleman's drink.</v>
       </c>
       <c r="C35" t="str">
-        <v>255 / 375 / 995</v>
+        <v>450</v>
       </c>
       <c r="D35" t="str">
-        <v>draught-beer</v>
+        <v>classic-cocktails</v>
       </c>
       <c r="E35" t="b">
         <v>1</v>
@@ -1218,16 +1218,16 @@
     </row>
     <row r="36">
       <c r="A36" t="str">
-        <v>Hoegaarden</v>
+        <v>Bloody Mary</v>
       </c>
       <c r="B36" t="str">
-        <v>Belgian wheat beer – smooth &amp; citrusy</v>
+        <v>Vodka, tomato juice, spice blend &amp; lemon. Savory, spicy &amp; energizing.</v>
       </c>
       <c r="C36" t="str">
-        <v>495</v>
+        <v>450</v>
       </c>
       <c r="D36" t="str">
-        <v>pint-beers</v>
+        <v>classic-cocktails</v>
       </c>
       <c r="E36" t="b">
         <v>1</v>
@@ -1241,16 +1241,16 @@
     </row>
     <row r="37">
       <c r="A37" t="str">
-        <v>Corona</v>
+        <v>Picante</v>
       </c>
       <c r="B37" t="str">
-        <v>Light &amp; crisp — best with lime</v>
+        <v>Tequila, lime &amp; chilli with a herbal twist. Fiery, bold &amp; addictive.</v>
       </c>
       <c r="C37" t="str">
-        <v>495</v>
+        <v>650</v>
       </c>
       <c r="D37" t="str">
-        <v>pint-beers</v>
+        <v>classic-cocktails</v>
       </c>
       <c r="E37" t="b">
         <v>1</v>
@@ -1264,16 +1264,16 @@
     </row>
     <row r="38">
       <c r="A38" t="str">
-        <v>Budweiser</v>
+        <v>Espresso Martini</v>
       </c>
       <c r="B38" t="str">
-        <v>Easy drinking lager</v>
+        <v>Vodka, coffee &amp; coffee liqueur. Rich, creamy &amp; caffeinated delight.</v>
       </c>
       <c r="C38" t="str">
-        <v>345</v>
+        <v>450</v>
       </c>
       <c r="D38" t="str">
-        <v>pint-beers</v>
+        <v>classic-cocktails</v>
       </c>
       <c r="E38" t="b">
         <v>1</v>
@@ -1287,16 +1287,16 @@
     </row>
     <row r="39">
       <c r="A39" t="str">
-        <v>Heineken</v>
+        <v>Daiquiri</v>
       </c>
       <c r="B39" t="str">
-        <v>Premium pilsner lager</v>
+        <v>Rum, lime &amp; sugar shaken crisp. Simple, sharp &amp; refreshing.</v>
       </c>
       <c r="C39" t="str">
-        <v>345</v>
+        <v>450</v>
       </c>
       <c r="D39" t="str">
-        <v>pint-beers</v>
+        <v>classic-cocktails</v>
       </c>
       <c r="E39" t="b">
         <v>1</v>
@@ -1310,10 +1310,10 @@
     </row>
     <row r="40">
       <c r="A40" t="str">
-        <v>Mojito</v>
+        <v>Negroni</v>
       </c>
       <c r="B40" t="str">
-        <v>Fresh mint, lime, sugar, and white rum topped with soda</v>
+        <v>Gin, sweet vermouth &amp; bitters. Bitter, complex &amp; beautifully balanced.</v>
       </c>
       <c r="C40" t="str">
         <v>450</v>
@@ -1333,10 +1333,10 @@
     </row>
     <row r="41">
       <c r="A41" t="str">
-        <v>Martini</v>
+        <v>Sidecar</v>
       </c>
       <c r="B41" t="str">
-        <v>Gin or vodka with dry vermouth</v>
+        <v>Brandy, triple sec &amp; lemon. Smooth citrus warmth.</v>
       </c>
       <c r="C41" t="str">
         <v>450</v>
@@ -1356,10 +1356,10 @@
     </row>
     <row r="42">
       <c r="A42" t="str">
-        <v>Margarita</v>
+        <v>Mai Tai</v>
       </c>
       <c r="B42" t="str">
-        <v>Tequila, lime &amp; triple sec with a salted rim</v>
+        <v>Rum, pineapple, lime &amp; almond. Exotic, fruity &amp; full-bodied.</v>
       </c>
       <c r="C42" t="str">
         <v>450</v>
@@ -1379,16 +1379,16 @@
     </row>
     <row r="43">
       <c r="A43" t="str">
-        <v>Manhattan</v>
+        <v>Summer's Clarity</v>
       </c>
       <c r="B43" t="str">
-        <v>Whisky stirred with sweet vermouth &amp; bitters</v>
+        <v>White rum with clarified watermelon, basil &amp; sparkle. Light, clean &amp; ultra refreshing.</v>
       </c>
       <c r="C43" t="str">
-        <v>450</v>
+        <v>595</v>
       </c>
       <c r="D43" t="str">
-        <v>classic-cocktails</v>
+        <v>signature-cocktails</v>
       </c>
       <c r="E43" t="b">
         <v>1</v>
@@ -1402,16 +1402,16 @@
     </row>
     <row r="44">
       <c r="A44" t="str">
-        <v>Old Fashioned</v>
+        <v>Azure Bloom</v>
       </c>
       <c r="B44" t="str">
-        <v>Whisky, bitter &amp; sugar, stirred on ice</v>
+        <v>Vodka, butterfly pea tea, mint &amp; airy carrot foam. Floral, vibrant &amp; visually stunning.</v>
       </c>
       <c r="C44" t="str">
-        <v>450</v>
+        <v>595</v>
       </c>
       <c r="D44" t="str">
-        <v>classic-cocktails</v>
+        <v>signature-cocktails</v>
       </c>
       <c r="E44" t="b">
         <v>1</v>
@@ -1425,10 +1425,10 @@
     </row>
     <row r="45">
       <c r="A45" t="str">
-        <v>Summer's Clarity</v>
+        <v>The Gilded Fig</v>
       </c>
       <c r="B45" t="str">
-        <v>White rum with clarified watermelon, basil &amp; sparkle</v>
+        <v>Brandy with aromatic wine reduction &amp; fig syrup. Rich, silky &amp; delicately sweet.</v>
       </c>
       <c r="C45" t="str">
         <v>595</v>
@@ -1448,10 +1448,10 @@
     </row>
     <row r="46">
       <c r="A46" t="str">
-        <v>Azure Bloom</v>
+        <v>The Mathri Merchant</v>
       </c>
       <c r="B46" t="str">
-        <v>Vodka, butterfly pea tea, mint &amp; airy carrot foam</v>
+        <v>Whisky, orange bitters, spiced syrup &amp; tea decoction. Warm, spiced &amp; culturally inspired.</v>
       </c>
       <c r="C46" t="str">
         <v>595</v>
@@ -1471,10 +1471,10 @@
     </row>
     <row r="47">
       <c r="A47" t="str">
-        <v>The Mathri Merchant</v>
+        <v>The Tangent Trail</v>
       </c>
       <c r="B47" t="str">
-        <v>Whisky, orange bitters, spiced syrup &amp; tea decoction</v>
+        <v>Tequila, spiced yuzu, pineapple &amp; milk clarification. Zesty, tropical &amp; crystal smooth.</v>
       </c>
       <c r="C47" t="str">
         <v>595</v>
@@ -1497,7 +1497,7 @@
         <v>Highland Tropical</v>
       </c>
       <c r="B48" t="str">
-        <v>Whisky, pineapple, banana syrup &amp; basil, milk-washed</v>
+        <v>Whisky, pineapple, banana syrup &amp; basil, milk-washed. Bold whisky meets tropical creaminess.</v>
       </c>
       <c r="C48" t="str">
         <v>595</v>
@@ -1520,7 +1520,7 @@
         <v>Midnight Nectar</v>
       </c>
       <c r="B49" t="str">
-        <v>Coconut-washed whisky, chocolate bitters &amp; jaggery</v>
+        <v>Coconut-washed whisky, chocolate bitters &amp; jaggery. Deep, exotic &amp; dessert-like.</v>
       </c>
       <c r="C49" t="str">
         <v>595</v>
@@ -1540,16 +1540,16 @@
     </row>
     <row r="50">
       <c r="A50" t="str">
-        <v>French 75</v>
+        <v>Indigo Bloom</v>
       </c>
       <c r="B50" t="str">
-        <v>Gin, lemon &amp; sparkling wine</v>
+        <v>Gin, butterfly pea tea, elderflower &amp; tonic. A floral, colour-changing beauty.</v>
       </c>
       <c r="C50" t="str">
-        <v>375</v>
+        <v>595</v>
       </c>
       <c r="D50" t="str">
-        <v>wine-cocktails</v>
+        <v>signature-cocktails</v>
       </c>
       <c r="E50" t="b">
         <v>1</v>
@@ -1563,16 +1563,16 @@
     </row>
     <row r="51">
       <c r="A51" t="str">
-        <v>Mimosa</v>
+        <v>The Crimson Glass</v>
       </c>
       <c r="B51" t="str">
-        <v>Orange juice topped with sparkling wine</v>
+        <v>Gin, cranberry, hibiscus &amp; milk clarity. Bright, tart &amp; silky smooth.</v>
       </c>
       <c r="C51" t="str">
-        <v>375</v>
+        <v>595</v>
       </c>
       <c r="D51" t="str">
-        <v>wine-cocktails</v>
+        <v>signature-cocktails</v>
       </c>
       <c r="E51" t="b">
         <v>1</v>
@@ -1586,16 +1586,16 @@
     </row>
     <row r="52">
       <c r="A52" t="str">
-        <v>Bellini</v>
+        <v>Black Sands Swizzle</v>
       </c>
       <c r="B52" t="str">
-        <v>Peach puree &amp; sparkling wine</v>
+        <v>White rum, charcoal, chilli bitters &amp; pineapple. Dark, dramatic &amp; deliciously bold.</v>
       </c>
       <c r="C52" t="str">
-        <v>375</v>
+        <v>595</v>
       </c>
       <c r="D52" t="str">
-        <v>wine-cocktails</v>
+        <v>signature-cocktails</v>
       </c>
       <c r="E52" t="b">
         <v>1</v>
@@ -1609,16 +1609,16 @@
     </row>
     <row r="53">
       <c r="A53" t="str">
-        <v>Spritzer</v>
+        <v>The Garden Fizz</v>
       </c>
       <c r="B53" t="str">
-        <v>White wine with soda</v>
+        <v>Vodka, vanilla, basil, sweet &amp; sour &amp; ginger ale. Fresh, fizzy &amp; aromatic.</v>
       </c>
       <c r="C53" t="str">
-        <v>375</v>
+        <v>595</v>
       </c>
       <c r="D53" t="str">
-        <v>wine-cocktails</v>
+        <v>signature-cocktails</v>
       </c>
       <c r="E53" t="b">
         <v>1</v>
@@ -1632,16 +1632,16 @@
     </row>
     <row r="54">
       <c r="A54" t="str">
-        <v>Red Sangria</v>
+        <v>The Midnight Affogato</v>
       </c>
       <c r="B54" t="str">
-        <v>Red wine, citrus fruits &amp; spices</v>
+        <v>Vodka, vanilla, coffee &amp; cream. A boozy dessert in a glass.</v>
       </c>
       <c r="C54" t="str">
-        <v>275 / 1200</v>
+        <v>595</v>
       </c>
       <c r="D54" t="str">
-        <v>sangria</v>
+        <v>signature-cocktails</v>
       </c>
       <c r="E54" t="b">
         <v>1</v>
@@ -1655,16 +1655,16 @@
     </row>
     <row r="55">
       <c r="A55" t="str">
-        <v>White Sangria</v>
+        <v>French 75</v>
       </c>
       <c r="B55" t="str">
-        <v>White wine with tropical fruits</v>
+        <v>Gin, lemon &amp; sparkling wine. Crisp, elegant &amp; bubbly.</v>
       </c>
       <c r="C55" t="str">
-        <v>275 / 1200</v>
+        <v>375</v>
       </c>
       <c r="D55" t="str">
-        <v>sangria</v>
+        <v>wine-cocktails</v>
       </c>
       <c r="E55" t="b">
         <v>1</v>
@@ -1678,16 +1678,16 @@
     </row>
     <row r="56">
       <c r="A56" t="str">
-        <v>7 Spirits Sangria</v>
+        <v>Mimosa</v>
       </c>
       <c r="B56" t="str">
-        <v>A powerful mix of wine &amp; four white spirits</v>
+        <v>Orange juice topped with sparkling wine. Brunch classic, light &amp; sunny.</v>
       </c>
       <c r="C56" t="str">
-        <v>425 / 1700</v>
+        <v>375</v>
       </c>
       <c r="D56" t="str">
-        <v>sangria</v>
+        <v>wine-cocktails</v>
       </c>
       <c r="E56" t="b">
         <v>1</v>
@@ -1701,16 +1701,16 @@
     </row>
     <row r="57">
       <c r="A57" t="str">
-        <v>Kamikaze</v>
+        <v>Spritzer</v>
       </c>
       <c r="B57" t="str">
-        <v>Signature shot</v>
+        <v>White wine with soda. Cool, low alcohol &amp; refreshing.</v>
       </c>
       <c r="C57" t="str">
-        <v>350 | Six: 1750</v>
+        <v>375</v>
       </c>
       <c r="D57" t="str">
-        <v>signature-shots</v>
+        <v>wine-cocktails</v>
       </c>
       <c r="E57" t="b">
         <v>1</v>
@@ -1724,16 +1724,16 @@
     </row>
     <row r="58">
       <c r="A58" t="str">
-        <v>B52</v>
+        <v>Bellini</v>
       </c>
       <c r="B58" t="str">
-        <v>Signature shot</v>
+        <v>Peach puree &amp; sparkling wine. Sweet, smooth &amp; celebratory.</v>
       </c>
       <c r="C58" t="str">
-        <v>400 | Six: 2000</v>
+        <v>375</v>
       </c>
       <c r="D58" t="str">
-        <v>signature-shots</v>
+        <v>wine-cocktails</v>
       </c>
       <c r="E58" t="b">
         <v>1</v>
@@ -1747,16 +1747,16 @@
     </row>
     <row r="59">
       <c r="A59" t="str">
-        <v>Jägerbomb</v>
+        <v>Marilyn Monroe</v>
       </c>
       <c r="B59" t="str">
-        <v>Signature shot</v>
+        <v>A glamorous sparkling wine cocktail with fruity notes. Sweet, soft &amp; iconic.</v>
       </c>
       <c r="C59" t="str">
-        <v>450 | Six: 2250</v>
+        <v>375</v>
       </c>
       <c r="D59" t="str">
-        <v>signature-shots</v>
+        <v>wine-cocktails</v>
       </c>
       <c r="E59" t="b">
         <v>1</v>
@@ -1770,16 +1770,16 @@
     </row>
     <row r="60">
       <c r="A60" t="str">
-        <v>Flaming Lamborghini</v>
+        <v>Barrel Bucket</v>
       </c>
       <c r="B60" t="str">
-        <v>Signature shot</v>
+        <v>Shareable, fun &amp; flavorful wine cocktails.</v>
       </c>
       <c r="C60" t="str">
-        <v>2000</v>
+        <v>900</v>
       </c>
       <c r="D60" t="str">
-        <v>signature-shots</v>
+        <v>wine-cocktails</v>
       </c>
       <c r="E60" t="b">
         <v>1</v>
@@ -1793,16 +1793,16 @@
     </row>
     <row r="61">
       <c r="A61" t="str">
-        <v>Johnnie Walker Black Label</v>
+        <v>Red Sangria</v>
       </c>
       <c r="B61" t="str">
-        <v>Premium blended Scotch whisky</v>
+        <v>Red wine, citrus fruits &amp; spices. Bold, fruity &amp; refreshing.</v>
       </c>
       <c r="C61" t="str">
-        <v>850</v>
+        <v>275 / 1200</v>
       </c>
       <c r="D61" t="str">
-        <v>blended-whisky</v>
+        <v>sangria</v>
       </c>
       <c r="E61" t="b">
         <v>1</v>
@@ -1816,16 +1816,16 @@
     </row>
     <row r="62">
       <c r="A62" t="str">
-        <v>Chivas Regal 12 Years</v>
+        <v>White Sangria</v>
       </c>
       <c r="B62" t="str">
-        <v>Smooth blended Scotch whisky</v>
+        <v>White wine with tropical fruits. Light, crisp &amp; summery.</v>
       </c>
       <c r="C62" t="str">
-        <v>900</v>
+        <v>275 / 1200</v>
       </c>
       <c r="D62" t="str">
-        <v>blended-whisky</v>
+        <v>sangria</v>
       </c>
       <c r="E62" t="b">
         <v>1</v>
@@ -1839,16 +1839,16 @@
     </row>
     <row r="63">
       <c r="A63" t="str">
-        <v>Glenmorangie Original</v>
+        <v>7 Spirits Sangria</v>
       </c>
       <c r="B63" t="str">
-        <v>Single malt Scotch whisky</v>
+        <v>A powerful mix of wine &amp; four white spirits. Stronger, richer &amp; party-ready.</v>
       </c>
       <c r="C63" t="str">
-        <v>950</v>
+        <v>425 / 1700</v>
       </c>
       <c r="D63" t="str">
-        <v>single-malt-whisky</v>
+        <v>sangria</v>
       </c>
       <c r="E63" t="b">
         <v>1</v>
@@ -1862,16 +1862,16 @@
     </row>
     <row r="64">
       <c r="A64" t="str">
-        <v>Macallan 12 Years</v>
+        <v>Double Bubble</v>
       </c>
       <c r="B64" t="str">
-        <v>Premium single malt whisky</v>
+        <v>Sparkling wine + fruity sangria blend. Fun, fizzy &amp; flavour-packed.</v>
       </c>
       <c r="C64" t="str">
-        <v>1200</v>
+        <v>425 / 1700</v>
       </c>
       <c r="D64" t="str">
-        <v>single-malt-whisky</v>
+        <v>sangria</v>
       </c>
       <c r="E64" t="b">
         <v>1</v>
@@ -1885,16 +1885,16 @@
     </row>
     <row r="65">
       <c r="A65" t="str">
-        <v>Balvenie DoubleWood</v>
+        <v>Kamikaze</v>
       </c>
       <c r="B65" t="str">
-        <v>Rich single malt Scotch whisky</v>
+        <v>Signature shot</v>
       </c>
       <c r="C65" t="str">
-        <v>1100</v>
+        <v>350 | Six: 1750</v>
       </c>
       <c r="D65" t="str">
-        <v>single-malt-whisky</v>
+        <v>signature-shots</v>
       </c>
       <c r="E65" t="b">
         <v>1</v>
@@ -1908,16 +1908,16 @@
     </row>
     <row r="66">
       <c r="A66" t="str">
-        <v>Jackass Broadside</v>
+        <v>B52</v>
       </c>
       <c r="B66" t="str">
-        <v>American Irish whiskey</v>
+        <v>Signature shot</v>
       </c>
       <c r="C66" t="str">
-        <v>850</v>
+        <v>400 | Six: 2000</v>
       </c>
       <c r="D66" t="str">
-        <v>american-irish-whiskey</v>
+        <v>signature-shots</v>
       </c>
       <c r="E66" t="b">
         <v>1</v>
@@ -1931,16 +1931,16 @@
     </row>
     <row r="67">
       <c r="A67" t="str">
-        <v>Blended Scotch Whisky</v>
+        <v>Jägerbomb</v>
       </c>
       <c r="B67" t="str">
-        <v>Classic blended whisky</v>
+        <v>Signature shot</v>
       </c>
       <c r="C67" t="str">
-        <v>750</v>
+        <v>450 | Six: 2250</v>
       </c>
       <c r="D67" t="str">
-        <v>blended-scotch-whisky</v>
+        <v>signature-shots</v>
       </c>
       <c r="E67" t="b">
         <v>1</v>
@@ -1954,16 +1954,16 @@
     </row>
     <row r="68">
       <c r="A68" t="str">
-        <v>Absolut Vodka</v>
+        <v>Mini Jägerbomb</v>
       </c>
       <c r="B68" t="str">
-        <v>Premium Swedish vodka</v>
+        <v>Signature shot (10 for 5)</v>
       </c>
       <c r="C68" t="str">
-        <v>750</v>
+        <v>1000 | 5000</v>
       </c>
       <c r="D68" t="str">
-        <v>vodka</v>
+        <v>signature-shots</v>
       </c>
       <c r="E68" t="b">
         <v>1</v>
@@ -1977,16 +1977,16 @@
     </row>
     <row r="69">
       <c r="A69" t="str">
-        <v>Tanqueray Gin</v>
+        <v>Lemon Drop</v>
       </c>
       <c r="B69" t="str">
-        <v>Classic London dry gin</v>
+        <v>Signature shot</v>
       </c>
       <c r="C69" t="str">
-        <v>850</v>
+        <v>350 | Six: 1750</v>
       </c>
       <c r="D69" t="str">
-        <v>gin</v>
+        <v>signature-shots</v>
       </c>
       <c r="E69" t="b">
         <v>1</v>
@@ -2000,16 +2000,16 @@
     </row>
     <row r="70">
       <c r="A70" t="str">
-        <v>Bacardi Rum</v>
+        <v>Monk Chocolate</v>
       </c>
       <c r="B70" t="str">
-        <v>Light premium rum</v>
+        <v>Signature shot</v>
       </c>
       <c r="C70" t="str">
-        <v>700</v>
+        <v>350 | Six: 1750</v>
       </c>
       <c r="D70" t="str">
-        <v>rum</v>
+        <v>signature-shots</v>
       </c>
       <c r="E70" t="b">
         <v>1</v>
@@ -2023,16 +2023,16 @@
     </row>
     <row r="71">
       <c r="A71" t="str">
-        <v>Jose Cuervo Tequila</v>
+        <v>Flaming Lamborghini</v>
       </c>
       <c r="B71" t="str">
-        <v>Traditional tequila</v>
+        <v>Signature shot</v>
       </c>
       <c r="C71" t="str">
-        <v>800</v>
+        <v>2000</v>
       </c>
       <c r="D71" t="str">
-        <v>tequila</v>
+        <v>signature-shots</v>
       </c>
       <c r="E71" t="b">
         <v>1</v>
@@ -2046,16 +2046,16 @@
     </row>
     <row r="72">
       <c r="A72" t="str">
-        <v>Hennessy Cognac</v>
+        <v>Fire Shot</v>
       </c>
       <c r="B72" t="str">
-        <v>Premium French cognac</v>
+        <v>Signature shot</v>
       </c>
       <c r="C72" t="str">
-        <v>1500</v>
+        <v>400 | Six: 2000</v>
       </c>
       <c r="D72" t="str">
-        <v>cognac-brandy</v>
+        <v>signature-shots</v>
       </c>
       <c r="E72" t="b">
         <v>1</v>
@@ -2064,472 +2064,12 @@
         <v/>
       </c>
       <c r="G72" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="73">
-      <c r="A73" t="str">
-        <v>Cointreau Liqueur</v>
-      </c>
-      <c r="B73" t="str">
-        <v>Premium triple sec liqueur</v>
-      </c>
-      <c r="C73" t="str">
-        <v>900</v>
-      </c>
-      <c r="D73" t="str">
-        <v>liqueurs</v>
-      </c>
-      <c r="E73" t="b">
-        <v>1</v>
-      </c>
-      <c r="F73" t="str">
-        <v/>
-      </c>
-      <c r="G73" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="74">
-      <c r="A74" t="str">
-        <v>Perrier-Jouet Champagne</v>
-      </c>
-      <c r="B74" t="str">
-        <v>Premium sparkling wine</v>
-      </c>
-      <c r="C74" t="str">
-        <v>2500</v>
-      </c>
-      <c r="D74" t="str">
-        <v>sparkling-wine</v>
-      </c>
-      <c r="E74" t="b">
-        <v>1</v>
-      </c>
-      <c r="F74" t="str">
-        <v/>
-      </c>
-      <c r="G74" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="75">
-      <c r="A75" t="str">
-        <v>Barefoot Sauvignon Blanc</v>
-      </c>
-      <c r="B75" t="str">
-        <v>Crisp white wine from California</v>
-      </c>
-      <c r="C75" t="str">
-        <v>1200</v>
-      </c>
-      <c r="D75" t="str">
-        <v>white-wines</v>
-      </c>
-      <c r="E75" t="b">
-        <v>1</v>
-      </c>
-      <c r="F75" t="str">
-        <v/>
-      </c>
-      <c r="G75" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="76">
-      <c r="A76" t="str">
-        <v>La Crema Chardonnay</v>
-      </c>
-      <c r="B76" t="str">
-        <v>Full-bodied white wine</v>
-      </c>
-      <c r="C76" t="str">
-        <v>1400</v>
-      </c>
-      <c r="D76" t="str">
-        <v>white-wines</v>
-      </c>
-      <c r="E76" t="b">
-        <v>1</v>
-      </c>
-      <c r="F76" t="str">
-        <v/>
-      </c>
-      <c r="G76" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="77">
-      <c r="A77" t="str">
-        <v>Sutter Home White Zinfandel</v>
-      </c>
-      <c r="B77" t="str">
-        <v>Sweet rose wine</v>
-      </c>
-      <c r="C77" t="str">
-        <v>1100</v>
-      </c>
-      <c r="D77" t="str">
-        <v>rose-wines</v>
-      </c>
-      <c r="E77" t="b">
-        <v>1</v>
-      </c>
-      <c r="F77" t="str">
-        <v/>
-      </c>
-      <c r="G77" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="78">
-      <c r="A78" t="str">
-        <v>Yellow Tail Cabernet Sauvignon</v>
-      </c>
-      <c r="B78" t="str">
-        <v>Rich red wine from Australia</v>
-      </c>
-      <c r="C78" t="str">
-        <v>1300</v>
-      </c>
-      <c r="D78" t="str">
-        <v>red-wines</v>
-      </c>
-      <c r="E78" t="b">
-        <v>1</v>
-      </c>
-      <c r="F78" t="str">
-        <v/>
-      </c>
-      <c r="G78" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="79">
-      <c r="A79" t="str">
-        <v>Barefoot Pinot Noir</v>
-      </c>
-      <c r="B79" t="str">
-        <v>Smooth red wine</v>
-      </c>
-      <c r="C79" t="str">
-        <v>1250</v>
-      </c>
-      <c r="D79" t="str">
-        <v>red-wines</v>
-      </c>
-      <c r="E79" t="b">
-        <v>1</v>
-      </c>
-      <c r="F79" t="str">
-        <v/>
-      </c>
-      <c r="G79" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="80">
-      <c r="A80" t="str">
-        <v>Bota Box Pinot Grigio</v>
-      </c>
-      <c r="B80" t="str">
-        <v>Affordable white wine box</v>
-      </c>
-      <c r="C80" t="str">
-        <v>950</v>
-      </c>
-      <c r="D80" t="str">
-        <v>white-wines</v>
-      </c>
-      <c r="E80" t="b">
-        <v>1</v>
-      </c>
-      <c r="F80" t="str">
-        <v/>
-      </c>
-      <c r="G80" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="81">
-      <c r="A81" t="str">
-        <v>Barefoot Red Blend</v>
-      </c>
-      <c r="B81" t="str">
-        <v>Fruit-forward red wine blend</v>
-      </c>
-      <c r="C81" t="str">
-        <v>1150</v>
-      </c>
-      <c r="D81" t="str">
-        <v>red-wines</v>
-      </c>
-      <c r="E81" t="b">
-        <v>1</v>
-      </c>
-      <c r="F81" t="str">
-        <v/>
-      </c>
-      <c r="G81" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="82">
-      <c r="A82" t="str">
-        <v>Barefoot Merlot</v>
-      </c>
-      <c r="B82" t="str">
-        <v>Smooth red wine</v>
-      </c>
-      <c r="C82" t="str">
-        <v>1200</v>
-      </c>
-      <c r="D82" t="str">
-        <v>red-wines</v>
-      </c>
-      <c r="E82" t="b">
-        <v>1</v>
-      </c>
-      <c r="F82" t="str">
-        <v/>
-      </c>
-      <c r="G82" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="83">
-      <c r="A83" t="str">
-        <v>Barefoot Cabernet Sauvignon</v>
-      </c>
-      <c r="B83" t="str">
-        <v>Bold red wine</v>
-      </c>
-      <c r="C83" t="str">
-        <v>1300</v>
-      </c>
-      <c r="D83" t="str">
-        <v>red-wines</v>
-      </c>
-      <c r="E83" t="b">
-        <v>1</v>
-      </c>
-      <c r="F83" t="str">
-        <v/>
-      </c>
-      <c r="G83" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="84">
-      <c r="A84" t="str">
-        <v>Taylor Dessert Wine</v>
-      </c>
-      <c r="B84" t="str">
-        <v>Sweet dessert wine</v>
-      </c>
-      <c r="C84" t="str">
-        <v>1100</v>
-      </c>
-      <c r="D84" t="str">
-        <v>dessert-wines</v>
-      </c>
-      <c r="E84" t="b">
-        <v>1</v>
-      </c>
-      <c r="F84" t="str">
-        <v/>
-      </c>
-      <c r="G84" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="85">
-      <c r="A85" t="str">
-        <v>Barefoot Zinfandel</v>
-      </c>
-      <c r="B85" t="str">
-        <v>Rich dessert wine</v>
-      </c>
-      <c r="C85" t="str">
-        <v>1250</v>
-      </c>
-      <c r="D85" t="str">
-        <v>dessert-wines</v>
-      </c>
-      <c r="E85" t="b">
-        <v>1</v>
-      </c>
-      <c r="F85" t="str">
-        <v/>
-      </c>
-      <c r="G85" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="86">
-      <c r="A86" t="str">
-        <v>Sandeman Tawny Port</v>
-      </c>
-      <c r="B86" t="str">
-        <v>Classic tawny port wine</v>
-      </c>
-      <c r="C86" t="str">
-        <v>1400</v>
-      </c>
-      <c r="D86" t="str">
-        <v>port-wine</v>
-      </c>
-      <c r="E86" t="b">
-        <v>1</v>
-      </c>
-      <c r="F86" t="str">
-        <v/>
-      </c>
-      <c r="G86" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="87">
-      <c r="A87" t="str">
-        <v>Barefoot Riesling</v>
-      </c>
-      <c r="B87" t="str">
-        <v>Semi-sweet white wine</v>
-      </c>
-      <c r="C87" t="str">
-        <v>1150</v>
-      </c>
-      <c r="D87" t="str">
-        <v>dessert-wines</v>
-      </c>
-      <c r="E87" t="b">
-        <v>1</v>
-      </c>
-      <c r="F87" t="str">
-        <v/>
-      </c>
-      <c r="G87" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="88">
-      <c r="A88" t="str">
-        <v>Mojito Mocktail</v>
-      </c>
-      <c r="B88" t="str">
-        <v>Fresh mint &amp; lime mocktail</v>
-      </c>
-      <c r="C88" t="str">
-        <v>250</v>
-      </c>
-      <c r="D88" t="str">
-        <v>signature-mocktails</v>
-      </c>
-      <c r="E88" t="b">
-        <v>1</v>
-      </c>
-      <c r="F88" t="str">
-        <v/>
-      </c>
-      <c r="G88" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="89">
-      <c r="A89" t="str">
-        <v>Virgin Margarita</v>
-      </c>
-      <c r="B89" t="str">
-        <v>Refreshing margarita without alcohol</v>
-      </c>
-      <c r="C89" t="str">
-        <v>250</v>
-      </c>
-      <c r="D89" t="str">
-        <v>signature-mocktails</v>
-      </c>
-      <c r="E89" t="b">
-        <v>1</v>
-      </c>
-      <c r="F89" t="str">
-        <v/>
-      </c>
-      <c r="G89" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="90">
-      <c r="A90" t="str">
-        <v>Lemonade</v>
-      </c>
-      <c r="B90" t="str">
-        <v>Fresh homemade lemonade</v>
-      </c>
-      <c r="C90" t="str">
-        <v>150</v>
-      </c>
-      <c r="D90" t="str">
-        <v>soft-beverages</v>
-      </c>
-      <c r="E90" t="b">
-        <v>1</v>
-      </c>
-      <c r="F90" t="str">
-        <v/>
-      </c>
-      <c r="G90" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="91">
-      <c r="A91" t="str">
-        <v>Iced Tea</v>
-      </c>
-      <c r="B91" t="str">
-        <v>Chilled iced tea</v>
-      </c>
-      <c r="C91" t="str">
-        <v>120</v>
-      </c>
-      <c r="D91" t="str">
-        <v>soft-beverages</v>
-      </c>
-      <c r="E91" t="b">
-        <v>1</v>
-      </c>
-      <c r="F91" t="str">
-        <v/>
-      </c>
-      <c r="G91" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="92">
-      <c r="A92" t="str">
-        <v>Mango Lassi</v>
-      </c>
-      <c r="B92" t="str">
-        <v>Traditional yogurt-based mango drink</v>
-      </c>
-      <c r="C92" t="str">
-        <v>180</v>
-      </c>
-      <c r="D92" t="str">
-        <v>soft-beverages</v>
-      </c>
-      <c r="E92" t="b">
-        <v>1</v>
-      </c>
-      <c r="F92" t="str">
-        <v/>
-      </c>
-      <c r="G92" t="b">
         <v>1</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:G92"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:G72"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Create a beverage-focused menu spreadsheet from text data
Attach a new spreadsheet file containing beverage and cocktail items, categorized and formatted according to the specified template.

Replit-Commit-Author: Agent
Replit-Commit-Session-Id: d5825b2d-5a70-4950-bc3e-e69072dc9210
Replit-Commit-Checkpoint-Type: full_checkpoint
Replit-Commit-Event-Id: 4da0cdce-d440-48b8-b3c7-a908d9811ce7
Replit-Commit-Screenshot-Url: https://storage.googleapis.com/screenshot-production-us-central1/a0e76cf1-50a4-4033-88e9-413827fbeca2/d5825b2d-5a70-4950-bc3e-e69072dc9210/hllg6Je
Replit-Helium-Checkpoint-Created: true
</commit_message>
<xml_diff>
--- a/BarrelBorn_Menu_Template.xlsx
+++ b/BarrelBorn_Menu_Template.xlsx
@@ -715,7 +715,7 @@
         <v>Kingfisher Strong</v>
       </c>
       <c r="B14" t="str">
-        <v>Strong &amp; popular lager</v>
+        <v>Strong &amp; popular</v>
       </c>
       <c r="C14" t="str">
         <v>375</v>
@@ -738,7 +738,7 @@
         <v>Budweiser Magnum</v>
       </c>
       <c r="B15" t="str">
-        <v>Strong &amp; popular lager</v>
+        <v>Strong &amp; popular</v>
       </c>
       <c r="C15" t="str">
         <v>435</v>
@@ -761,7 +761,7 @@
         <v>Carlsberg Elephant</v>
       </c>
       <c r="B16" t="str">
-        <v>Strong &amp; popular lager</v>
+        <v>Strong &amp; popular</v>
       </c>
       <c r="C16" t="str">
         <v>375</v>
@@ -784,7 +784,7 @@
         <v>Budweiser</v>
       </c>
       <c r="B17" t="str">
-        <v>Easy drinking lager</v>
+        <v>Easy drinking</v>
       </c>
       <c r="C17" t="str">
         <v>345</v>
@@ -807,7 +807,7 @@
         <v>Amstel Light</v>
       </c>
       <c r="B18" t="str">
-        <v>Easy drinking lager</v>
+        <v>Easy drinking</v>
       </c>
       <c r="C18" t="str">
         <v>375</v>
@@ -830,7 +830,7 @@
         <v>Carlsberg Smooth</v>
       </c>
       <c r="B19" t="str">
-        <v>Easy drinking lager</v>
+        <v>Easy drinking</v>
       </c>
       <c r="C19" t="str">
         <v>345</v>
@@ -853,7 +853,7 @@
         <v>Heineken</v>
       </c>
       <c r="B20" t="str">
-        <v>Easy drinking lager</v>
+        <v>Easy drinking</v>
       </c>
       <c r="C20" t="str">
         <v>345</v>
@@ -1014,7 +1014,7 @@
         <v>LIIT</v>
       </c>
       <c r="B27" t="str">
-        <v>Powerful blend of five white spirits, citrus, and cola. Our strongest classic.</v>
+        <v>A powerful blend of five white spirits, citrus, and cola. Our strongest classic.</v>
       </c>
       <c r="C27" t="str">
         <v>800</v>
@@ -1773,7 +1773,7 @@
         <v>Barrel Bucket</v>
       </c>
       <c r="B60" t="str">
-        <v>Shareable, fun &amp; flavorful wine cocktails.</v>
+        <v>Shareable, fun &amp; flavorful wine cocktails</v>
       </c>
       <c r="C60" t="str">
         <v>900</v>

</xml_diff>